<commit_message>
actualizo informe aplicada, me olvide de cambiar el circuito del balanceo doble
</commit_message>
<xml_diff>
--- a/Electronica Aplicada 3/TP's/TPN3/Informe/tablas/CPL2.xlsx
+++ b/Electronica Aplicada 3/TP's/TPN3/Informe/tablas/CPL2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fnavarro\5to\Electronica Aplicada 3\TP's\TPN3\Informe\tablas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{753FEBAD-F9E6-44AD-BD83-F4CD5A67DC09}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9068B75C-ABC0-4D41-B02A-5E445D26DD26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{679CE008-933A-46CB-A0FF-8E305BB9A0F6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{679CE008-933A-46CB-A0FF-8E305BB9A0F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -45,8 +45,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -86,10 +94,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC35CEF6-72E1-4836-B4D7-B36F36EEACF2}">
-  <dimension ref="A1:E252"/>
+  <dimension ref="A1:H252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="C182" sqref="C182"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="H85" sqref="H85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,15 +437,15 @@
         <v>-5</v>
       </c>
       <c r="B2">
-        <v>-21.771699999999999</v>
+        <v>-17.049900000000001</v>
       </c>
       <c r="C2">
-        <f>((142/175)*A2) -18.12</f>
-        <v>-22.177142857142858</v>
+        <f>((104/125)*A2) -12.89</f>
+        <v>-17.05</v>
       </c>
       <c r="E2">
         <f>C2-B2</f>
-        <v>-0.40544285714285877</v>
+        <v>-9.9999999999766942E-5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -444,15 +453,15 @@
         <v>-4.9000000000000004</v>
       </c>
       <c r="B3">
-        <v>-21.699000000000002</v>
+        <v>-16.966899999999999</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C66" si="0">((142/175)*A3) -18.12</f>
-        <v>-22.096</v>
+        <f t="shared" ref="C3:C66" si="0">((104/125)*A3) -12.89</f>
+        <v>-16.966799999999999</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E66" si="1">C3-B3</f>
-        <v>-0.39699999999999847</v>
+        <v>9.9999999999766942E-5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -460,15 +469,15 @@
         <v>-4.8</v>
       </c>
       <c r="B4">
-        <v>-21.626000000000001</v>
+        <v>-16.883800000000001</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>-22.014857142857142</v>
+        <v>-16.883600000000001</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>-0.38885714285714101</v>
+        <v>1.9999999999953388E-4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -476,15 +485,15 @@
         <v>-4.7</v>
       </c>
       <c r="B5">
-        <v>-21.5535</v>
+        <v>-16.800799999999999</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>-21.933714285714288</v>
+        <v>-16.8004</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>-0.38021428571428828</v>
+        <v>3.9999999999906777E-4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -492,15 +501,15 @@
         <v>-4.5999999999999996</v>
       </c>
       <c r="B6">
-        <v>-21.481100000000001</v>
+        <v>-16.717700000000001</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>-21.85257142857143</v>
+        <v>-16.717199999999998</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>-0.37147142857142867</v>
+        <v>5.0000000000238742E-4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -508,15 +517,15 @@
         <v>-4.5</v>
       </c>
       <c r="B7">
-        <v>-21.408999999999999</v>
+        <v>-16.634699999999999</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>-21.771428571428572</v>
+        <v>-16.634</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>-0.36242857142857332</v>
+        <v>6.9999999999836859E-4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -524,15 +533,15 @@
         <v>-4.4000000000000004</v>
       </c>
       <c r="B8">
-        <v>-21.3371</v>
+        <v>-16.551600000000001</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>-21.690285714285714</v>
+        <v>-16.550800000000002</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>-0.35318571428571488</v>
+        <v>7.9999999999813554E-4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -540,15 +549,15 @@
         <v>-4.3</v>
       </c>
       <c r="B9">
-        <v>-21.2654</v>
+        <v>-16.468499999999999</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>-21.609142857142857</v>
+        <v>-16.467600000000001</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>-0.34374285714285691</v>
+        <v>8.9999999999790248E-4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -556,15 +565,15 @@
         <v>-4.2</v>
       </c>
       <c r="B10">
-        <v>-21.193899999999999</v>
+        <v>-16.385300000000001</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>-21.528000000000002</v>
+        <v>-16.384399999999999</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>-0.33410000000000295</v>
+        <v>9.0000000000145519E-4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -572,15 +581,15 @@
         <v>-4.0999999999999996</v>
       </c>
       <c r="B11">
-        <v>-21.122499999999999</v>
+        <v>-16.302199999999999</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>-21.446857142857144</v>
+        <v>-16.301200000000001</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>-0.32435714285714567</v>
+        <v>9.9999999999766942E-4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -588,15 +597,15 @@
         <v>-4</v>
       </c>
       <c r="B12">
-        <v>-21.051300000000001</v>
+        <v>-16.219000000000001</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>-21.365714285714287</v>
+        <v>-16.218</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>-0.31441428571428531</v>
+        <v>1.0000000000012221E-3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -604,15 +613,15 @@
         <v>-3.9</v>
       </c>
       <c r="B13">
-        <v>-20.9803</v>
+        <v>-16.1358</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>-21.284571428571429</v>
+        <v>-16.134799999999998</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>-0.30427142857142897</v>
+        <v>1.0000000000012221E-3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -620,15 +629,15 @@
         <v>-3.8</v>
       </c>
       <c r="B14">
-        <v>-20.909500000000001</v>
+        <v>-16.052600000000002</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>-21.203428571428571</v>
+        <v>-16.051600000000001</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>-0.29392857142856954</v>
+        <v>1.0000000000012221E-3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -636,15 +645,15 @@
         <v>-3.7</v>
       </c>
       <c r="B15">
-        <v>-20.838699999999999</v>
+        <v>-15.9695</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>-21.122285714285717</v>
+        <v>-15.968400000000001</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>-0.28358571428571722</v>
+        <v>1.0999999999992127E-3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -652,15 +661,15 @@
         <v>-3.6</v>
       </c>
       <c r="B16">
-        <v>-20.765699999999999</v>
+        <v>-15.8847</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>-21.041142857142859</v>
+        <v>-15.885200000000001</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>-0.27544285714285976</v>
+        <v>-5.0000000000061107E-4</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -668,15 +677,15 @@
         <v>-3.5</v>
       </c>
       <c r="B17">
-        <v>-20.694600000000001</v>
+        <v>-15.8011</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>-20.96</v>
+        <v>-15.802</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>-0.26539999999999964</v>
+        <v>-8.9999999999967883E-4</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -684,15 +693,15 @@
         <v>-3.4</v>
       </c>
       <c r="B18">
-        <v>-20.6235</v>
+        <v>-15.7174</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>-20.878857142857143</v>
+        <v>-15.7188</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>-0.25535714285714306</v>
+        <v>-1.4000000000002899E-3</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -700,15 +709,15 @@
         <v>-3.3</v>
       </c>
       <c r="B19">
-        <v>-20.552299999999999</v>
+        <v>-15.633599999999999</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>-20.797714285714285</v>
+        <v>-15.6356</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>-0.24541428571428625</v>
+        <v>-2.0000000000006679E-3</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -716,15 +725,15 @@
         <v>-3.2</v>
       </c>
       <c r="B20">
-        <v>-20.481200000000001</v>
+        <v>-15.549799999999999</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>-20.716571428571431</v>
+        <v>-15.5524</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
-        <v>-0.23537142857142968</v>
+        <v>-2.6000000000010459E-3</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -732,15 +741,15 @@
         <v>-3.1</v>
       </c>
       <c r="B21">
-        <v>-20.41</v>
+        <v>-15.4659</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>-20.635428571428573</v>
+        <v>-15.469200000000001</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
-        <v>-0.22542857142857287</v>
+        <v>-3.3000000000011909E-3</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -748,15 +757,15 @@
         <v>-3</v>
       </c>
       <c r="B22">
-        <v>-20.338799999999999</v>
+        <v>-15.382</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>-20.554285714285715</v>
+        <v>-15.386000000000001</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
-        <v>-0.21548571428571606</v>
+        <v>-4.0000000000013358E-3</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -764,15 +773,15 @@
         <v>-2.9</v>
       </c>
       <c r="B23">
-        <v>-20.267499999999998</v>
+        <v>-15.298</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>-20.473142857142857</v>
+        <v>-15.302800000000001</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
-        <v>-0.20564285714285901</v>
+        <v>-4.8000000000012477E-3</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -780,15 +789,15 @@
         <v>-2.8</v>
       </c>
       <c r="B24">
-        <v>-20.196200000000001</v>
+        <v>-15.214</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>-20.391999999999999</v>
+        <v>-15.2196</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
-        <v>-0.19579999999999842</v>
+        <v>-5.5999999999993832E-3</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -796,15 +805,15 @@
         <v>-2.7</v>
       </c>
       <c r="B25">
-        <v>-20.1248</v>
+        <v>-15.129899999999999</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>-20.310857142857145</v>
+        <v>-15.1364</v>
       </c>
       <c r="E25">
         <f t="shared" si="1"/>
-        <v>-0.1860571428571447</v>
+        <v>-6.5000000000008384E-3</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -812,15 +821,15 @@
         <v>-2.6</v>
       </c>
       <c r="B26">
-        <v>-20.0533</v>
+        <v>-15.0458</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>-20.229714285714287</v>
+        <v>-15.0532</v>
       </c>
       <c r="E26">
         <f t="shared" si="1"/>
-        <v>-0.17641428571428719</v>
+        <v>-7.4000000000005173E-3</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -828,15 +837,15 @@
         <v>-2.5</v>
       </c>
       <c r="B27">
-        <v>-19.9817</v>
+        <v>-14.9618</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>-20.148571428571429</v>
+        <v>-14.97</v>
       </c>
       <c r="E27">
         <f t="shared" si="1"/>
-        <v>-0.16687142857142945</v>
+        <v>-8.2000000000004292E-3</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -844,15 +853,15 @@
         <v>-2.4</v>
       </c>
       <c r="B28">
-        <v>-19.9101</v>
+        <v>-14.877700000000001</v>
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>-20.067428571428572</v>
+        <v>-14.886800000000001</v>
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
-        <v>-0.15732857142857171</v>
+        <v>-9.100000000000108E-3</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -860,15 +869,15 @@
         <v>-2.2999999999999998</v>
       </c>
       <c r="B29">
-        <v>-19.8383</v>
+        <v>-14.792199999999999</v>
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>-19.986285714285714</v>
+        <v>-14.803599999999999</v>
       </c>
       <c r="E29">
         <f t="shared" si="1"/>
-        <v>-0.1479857142857135</v>
+        <v>-1.1400000000000077E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -876,15 +885,15 @@
         <v>-2.2000000000000002</v>
       </c>
       <c r="B30">
-        <v>-19.766400000000001</v>
+        <v>-14.707800000000001</v>
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>-19.905142857142859</v>
+        <v>-14.720400000000001</v>
       </c>
       <c r="E30">
         <f t="shared" si="1"/>
-        <v>-0.13874285714285861</v>
+        <v>-1.2600000000000833E-2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -892,15 +901,15 @@
         <v>-2.1</v>
       </c>
       <c r="B31">
-        <v>-19.694500000000001</v>
+        <v>-14.6234</v>
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>-19.824000000000002</v>
+        <v>-14.6372</v>
       </c>
       <c r="E31">
         <f t="shared" si="1"/>
-        <v>-0.12950000000000017</v>
+        <v>-1.3799999999999812E-2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -908,15 +917,15 @@
         <v>-2</v>
       </c>
       <c r="B32">
-        <v>-19.622399999999999</v>
+        <v>-14.5389</v>
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>-19.742857142857144</v>
+        <v>-14.554</v>
       </c>
       <c r="E32">
         <f t="shared" si="1"/>
-        <v>-0.12045714285714482</v>
+        <v>-1.5100000000000335E-2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -924,15 +933,15 @@
         <v>-1.9</v>
       </c>
       <c r="B33">
-        <v>-19.548100000000002</v>
+        <v>-14.454499999999999</v>
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>-19.661714285714286</v>
+        <v>-14.470800000000001</v>
       </c>
       <c r="E33">
         <f t="shared" si="1"/>
-        <v>-0.11361428571428434</v>
+        <v>-1.6300000000001091E-2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -940,15 +949,15 @@
         <v>-1.8</v>
       </c>
       <c r="B34">
-        <v>-19.475300000000001</v>
+        <v>-14.37</v>
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>-19.580571428571428</v>
+        <v>-14.387600000000001</v>
       </c>
       <c r="E34">
         <f t="shared" si="1"/>
-        <v>-0.10527142857142735</v>
+        <v>-1.7600000000001614E-2</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -956,15 +965,15 @@
         <v>-1.7</v>
       </c>
       <c r="B35">
-        <v>-19.4024</v>
+        <v>-14.285600000000001</v>
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>-19.499428571428574</v>
+        <v>-14.304400000000001</v>
       </c>
       <c r="E35">
         <f t="shared" si="1"/>
-        <v>-9.7028571428573684E-2</v>
+        <v>-1.8800000000000594E-2</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -972,15 +981,15 @@
         <v>-1.6</v>
       </c>
       <c r="B36">
-        <v>-19.3292</v>
+        <v>-14.2013</v>
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
-        <v>-19.418285714285716</v>
+        <v>-14.2212</v>
       </c>
       <c r="E36">
         <f t="shared" si="1"/>
-        <v>-8.9085714285715767E-2</v>
+        <v>-1.9899999999999807E-2</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -988,15 +997,15 @@
         <v>-1.5</v>
       </c>
       <c r="B37">
-        <v>-19.255800000000001</v>
+        <v>-14.117000000000001</v>
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
-        <v>-19.337142857142858</v>
+        <v>-14.138</v>
       </c>
       <c r="E37">
         <f t="shared" si="1"/>
-        <v>-8.1342857142857383E-2</v>
+        <v>-2.0999999999999019E-2</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1004,15 +1013,15 @@
         <v>-1.4</v>
       </c>
       <c r="B38">
-        <v>-19.182099999999998</v>
+        <v>-14.0329</v>
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
-        <v>-19.256</v>
+        <v>-14.0548</v>
       </c>
       <c r="E38">
         <f t="shared" si="1"/>
-        <v>-7.3900000000001853E-2</v>
+        <v>-2.1900000000000475E-2</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1020,15 +1029,15 @@
         <v>-1.3</v>
       </c>
       <c r="B39">
-        <v>-19.1083</v>
+        <v>-13.949</v>
       </c>
       <c r="C39">
         <f t="shared" si="0"/>
-        <v>-19.174857142857142</v>
+        <v>-13.9716</v>
       </c>
       <c r="E39">
         <f t="shared" si="1"/>
-        <v>-6.6557142857142537E-2</v>
+        <v>-2.260000000000062E-2</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1036,15 +1045,15 @@
         <v>-1.2</v>
       </c>
       <c r="B40">
-        <v>-19.034199999999998</v>
+        <v>-13.8642</v>
       </c>
       <c r="C40">
         <f t="shared" si="0"/>
-        <v>-19.093714285714288</v>
+        <v>-13.888400000000001</v>
       </c>
       <c r="E40">
         <f t="shared" si="1"/>
-        <v>-5.9514285714289628E-2</v>
+        <v>-2.4200000000000443E-2</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1052,15 +1061,15 @@
         <v>-1.1000000000000001</v>
       </c>
       <c r="B41">
-        <v>-18.959900000000001</v>
+        <v>-13.7804</v>
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
-        <v>-19.01257142857143</v>
+        <v>-13.805200000000001</v>
       </c>
       <c r="E41">
         <f t="shared" si="1"/>
-        <v>-5.2671428571429146E-2</v>
+        <v>-2.4800000000000821E-2</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1068,15 +1077,15 @@
         <v>-1</v>
       </c>
       <c r="B42">
-        <v>-18.885400000000001</v>
+        <v>-13.6967</v>
       </c>
       <c r="C42">
         <f t="shared" si="0"/>
-        <v>-18.931428571428572</v>
+        <v>-13.722000000000001</v>
       </c>
       <c r="E42">
         <f t="shared" si="1"/>
-        <v>-4.6028571428571752E-2</v>
+        <v>-2.5300000000001432E-2</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1084,15 +1093,15 @@
         <v>-0.9</v>
       </c>
       <c r="B43">
-        <v>-18.810700000000001</v>
+        <v>-13.6134</v>
       </c>
       <c r="C43">
         <f t="shared" si="0"/>
-        <v>-18.850285714285715</v>
+        <v>-13.6388</v>
       </c>
       <c r="E43">
         <f t="shared" si="1"/>
-        <v>-3.9585714285713891E-2</v>
+        <v>-2.5399999999999423E-2</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1100,15 +1109,15 @@
         <v>-0.8</v>
       </c>
       <c r="B44">
-        <v>-18.735700000000001</v>
+        <v>-13.5303</v>
       </c>
       <c r="C44">
         <f t="shared" si="0"/>
-        <v>-18.769142857142857</v>
+        <v>-13.5556</v>
       </c>
       <c r="E44">
         <f t="shared" si="1"/>
-        <v>-3.3442857142855331E-2</v>
+        <v>-2.5299999999999656E-2</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1116,15 +1125,15 @@
         <v>-0.7</v>
       </c>
       <c r="B45">
-        <v>-18.660499999999999</v>
+        <v>-13.4476</v>
       </c>
       <c r="C45">
         <f t="shared" si="0"/>
-        <v>-18.688000000000002</v>
+        <v>-13.4724</v>
       </c>
       <c r="E45">
         <f t="shared" si="1"/>
-        <v>-2.7500000000003411E-2</v>
+        <v>-2.4800000000000821E-2</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1132,15 +1141,15 @@
         <v>-0.6</v>
       </c>
       <c r="B46">
-        <v>-18.585000000000001</v>
+        <v>-13.365399999999999</v>
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
-        <v>-18.606857142857145</v>
+        <v>-13.389200000000001</v>
       </c>
       <c r="E46">
         <f t="shared" si="1"/>
-        <v>-2.1857142857143685E-2</v>
+        <v>-2.3800000000001376E-2</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1148,15 +1157,15 @@
         <v>-0.5</v>
       </c>
       <c r="B47">
-        <v>-18.509399999999999</v>
+        <v>-13.2837</v>
       </c>
       <c r="C47">
         <f t="shared" si="0"/>
-        <v>-18.525714285714287</v>
+        <v>-13.306000000000001</v>
       </c>
       <c r="E47">
         <f t="shared" si="1"/>
-        <v>-1.631428571428728E-2</v>
+        <v>-2.2300000000001319E-2</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1164,15 +1173,15 @@
         <v>-0.4</v>
       </c>
       <c r="B48">
-        <v>-18.432300000000001</v>
+        <v>-13.2027</v>
       </c>
       <c r="C48">
         <f t="shared" si="0"/>
-        <v>-18.444571428571429</v>
+        <v>-13.222800000000001</v>
       </c>
       <c r="E48">
         <f t="shared" si="1"/>
-        <v>-1.2271428571427379E-2</v>
+        <v>-2.0100000000001117E-2</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1180,15 +1189,15 @@
         <v>-0.3</v>
       </c>
       <c r="B49">
-        <v>-18.355899999999998</v>
+        <v>-13.122400000000001</v>
       </c>
       <c r="C49">
         <f t="shared" si="0"/>
-        <v>-18.363428571428571</v>
+        <v>-13.1396</v>
       </c>
       <c r="E49">
         <f t="shared" si="1"/>
-        <v>-7.5285714285726613E-3</v>
+        <v>-1.7199999999998994E-2</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1196,15 +1205,15 @@
         <v>-0.2</v>
       </c>
       <c r="B50">
-        <v>-18.279199999999999</v>
+        <v>-13.042899999999999</v>
       </c>
       <c r="C50">
         <f t="shared" si="0"/>
-        <v>-18.282285714285717</v>
+        <v>-13.0564</v>
       </c>
       <c r="E50">
         <f t="shared" si="1"/>
-        <v>-3.0857142857172448E-3</v>
+        <v>-1.3500000000000512E-2</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1212,15 +1221,15 @@
         <v>-0.1</v>
       </c>
       <c r="B51">
-        <v>-18.202200000000001</v>
+        <v>-12.964399999999999</v>
       </c>
       <c r="C51">
         <f t="shared" si="0"/>
-        <v>-18.201142857142859</v>
+        <v>-12.9732</v>
       </c>
       <c r="E51">
         <f t="shared" si="1"/>
-        <v>1.0571428571424235E-3</v>
+        <v>-8.8000000000008072E-3</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1228,15 +1237,15 @@
         <v>0</v>
       </c>
       <c r="B52">
-        <v>-18.1249</v>
+        <v>-12.8871</v>
       </c>
       <c r="C52">
         <f t="shared" si="0"/>
-        <v>-18.12</v>
+        <v>-12.89</v>
       </c>
       <c r="E52">
         <f t="shared" si="1"/>
-        <v>4.8999999999992383E-3</v>
+        <v>-2.9000000000003467E-3</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1244,15 +1253,15 @@
         <v>0.1</v>
       </c>
       <c r="B53">
-        <v>-18.0474</v>
+        <v>-12.811</v>
       </c>
       <c r="C53">
         <f t="shared" si="0"/>
-        <v>-18.038857142857143</v>
+        <v>-12.806800000000001</v>
       </c>
       <c r="E53">
         <f t="shared" si="1"/>
-        <v>8.5428571428565192E-3</v>
+        <v>4.1999999999990933E-3</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1260,15 +1269,15 @@
         <v>0.2</v>
       </c>
       <c r="B54">
-        <v>-17.9695</v>
+        <v>-12.7362</v>
       </c>
       <c r="C54">
         <f t="shared" si="0"/>
-        <v>-17.957714285714285</v>
+        <v>-12.723600000000001</v>
       </c>
       <c r="E54">
         <f t="shared" si="1"/>
-        <v>1.1785714285714732E-2</v>
+        <v>1.2599999999999056E-2</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1276,15 +1285,15 @@
         <v>0.3</v>
       </c>
       <c r="B55">
-        <v>-17.891400000000001</v>
+        <v>-12.663</v>
       </c>
       <c r="C55">
         <f t="shared" si="0"/>
-        <v>-17.876571428571431</v>
+        <v>-12.640400000000001</v>
       </c>
       <c r="E55">
         <f t="shared" si="1"/>
-        <v>1.4828571428569859E-2</v>
+        <v>2.2599999999998843E-2</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -1292,15 +1301,15 @@
         <v>0.4</v>
       </c>
       <c r="B56">
-        <v>-17.812999999999999</v>
+        <v>-12.5914</v>
       </c>
       <c r="C56">
         <f t="shared" si="0"/>
-        <v>-17.795428571428573</v>
+        <v>-12.5572</v>
       </c>
       <c r="E56">
         <f t="shared" si="1"/>
-        <v>1.7571428571425685E-2</v>
+        <v>3.420000000000023E-2</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -1308,15 +1317,15 @@
         <v>0.5</v>
       </c>
       <c r="B57">
-        <v>-17.734400000000001</v>
+        <v>-12.5214</v>
       </c>
       <c r="C57">
         <f t="shared" si="0"/>
-        <v>-17.714285714285715</v>
+        <v>-12.474</v>
       </c>
       <c r="E57">
         <f t="shared" si="1"/>
-        <v>2.0114285714285529E-2</v>
+        <v>4.7399999999999665E-2</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1324,15 +1333,15 @@
         <v>0.6</v>
       </c>
       <c r="B58">
-        <v>-17.6554</v>
+        <v>-12.4526</v>
       </c>
       <c r="C58">
         <f t="shared" si="0"/>
-        <v>-17.633142857142857</v>
+        <v>-12.3908</v>
       </c>
       <c r="E58">
         <f t="shared" si="1"/>
-        <v>2.2257142857142753E-2</v>
+        <v>6.1799999999999855E-2</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1340,15 +1349,15 @@
         <v>0.7</v>
       </c>
       <c r="B59">
-        <v>-17.5762</v>
+        <v>-12.386100000000001</v>
       </c>
       <c r="C59">
         <f t="shared" si="0"/>
-        <v>-17.552</v>
+        <v>-12.307600000000001</v>
       </c>
       <c r="E59">
         <f t="shared" si="1"/>
-        <v>2.4200000000000443E-2</v>
+        <v>7.8500000000000014E-2</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -1356,15 +1365,15 @@
         <v>0.8</v>
       </c>
       <c r="B60">
-        <v>-17.4968</v>
+        <v>-12.321300000000001</v>
       </c>
       <c r="C60">
         <f t="shared" si="0"/>
-        <v>-17.470857142857145</v>
+        <v>-12.224400000000001</v>
       </c>
       <c r="E60">
         <f t="shared" si="1"/>
-        <v>2.5942857142855047E-2</v>
+        <v>9.6899999999999764E-2</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -1372,15 +1381,15 @@
         <v>0.9</v>
       </c>
       <c r="B61">
-        <v>-17.416399999999999</v>
+        <v>-12.2585</v>
       </c>
       <c r="C61">
         <f t="shared" si="0"/>
-        <v>-17.389714285714287</v>
+        <v>-12.141200000000001</v>
       </c>
       <c r="E61">
         <f t="shared" si="1"/>
-        <v>2.6685714285711981E-2</v>
+        <v>0.11729999999999841</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -1388,15 +1397,15 @@
         <v>1</v>
       </c>
       <c r="B62">
-        <v>-17.336300000000001</v>
+        <v>-12.1974</v>
       </c>
       <c r="C62">
         <f t="shared" si="0"/>
-        <v>-17.30857142857143</v>
+        <v>-12.058</v>
       </c>
       <c r="E62">
         <f t="shared" si="1"/>
-        <v>2.7728571428571769E-2</v>
+        <v>0.13940000000000019</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -1404,15 +1413,15 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B63">
-        <v>-17.255800000000001</v>
+        <v>-12.138</v>
       </c>
       <c r="C63">
         <f t="shared" si="0"/>
-        <v>-17.227428571428572</v>
+        <v>-11.9748</v>
       </c>
       <c r="E63">
         <f t="shared" si="1"/>
-        <v>2.8371428571428936E-2</v>
+        <v>0.16319999999999979</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -1420,15 +1429,15 @@
         <v>1.2</v>
       </c>
       <c r="B64">
-        <v>-17.1751</v>
+        <v>-12.080500000000001</v>
       </c>
       <c r="C64">
         <f t="shared" si="0"/>
-        <v>-17.146285714285714</v>
+        <v>-11.8916</v>
       </c>
       <c r="E64">
         <f t="shared" si="1"/>
-        <v>2.8814285714286569E-2</v>
+        <v>0.18890000000000029</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -1436,15 +1445,15 @@
         <v>1.3</v>
       </c>
       <c r="B65">
-        <v>-17.094100000000001</v>
+        <v>-12.024699999999999</v>
       </c>
       <c r="C65">
         <f t="shared" si="0"/>
-        <v>-17.06514285714286</v>
+        <v>-11.808400000000001</v>
       </c>
       <c r="E65">
         <f t="shared" si="1"/>
-        <v>2.8957142857141349E-2</v>
+        <v>0.2162999999999986</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -1452,15 +1461,15 @@
         <v>1.4</v>
       </c>
       <c r="B66">
-        <v>-17.012799999999999</v>
+        <v>-11.970599999999999</v>
       </c>
       <c r="C66">
         <f t="shared" si="0"/>
-        <v>-16.984000000000002</v>
+        <v>-11.725200000000001</v>
       </c>
       <c r="E66">
         <f t="shared" si="1"/>
-        <v>2.8799999999996828E-2</v>
+        <v>0.24539999999999829</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -1468,15 +1477,15 @@
         <v>1.5</v>
       </c>
       <c r="B67">
-        <v>-16.9312</v>
+        <v>-11.9183</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:C130" si="2">((142/175)*A67) -18.12</f>
-        <v>-16.902857142857144</v>
+        <f t="shared" ref="C67:C130" si="2">((104/125)*A67) -12.89</f>
+        <v>-11.642000000000001</v>
       </c>
       <c r="E67">
         <f t="shared" ref="E67:E130" si="3">C67-B67</f>
-        <v>2.8342857142856559E-2</v>
+        <v>0.2762999999999991</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -1484,15 +1493,15 @@
         <v>1.6</v>
       </c>
       <c r="B68">
-        <v>-16.849399999999999</v>
+        <v>-11.867699999999999</v>
       </c>
       <c r="C68">
         <f t="shared" si="2"/>
-        <v>-16.821714285714286</v>
+        <v>-11.558800000000002</v>
       </c>
       <c r="E68">
         <f t="shared" si="3"/>
-        <v>2.7685714285713203E-2</v>
+        <v>0.30889999999999773</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -1500,15 +1509,15 @@
         <v>1.7</v>
       </c>
       <c r="B69">
-        <v>-16.767299999999999</v>
+        <v>-11.8187</v>
       </c>
       <c r="C69">
         <f t="shared" si="2"/>
-        <v>-16.740571428571428</v>
+        <v>-11.4756</v>
       </c>
       <c r="E69">
         <f t="shared" si="3"/>
-        <v>2.6728571428570547E-2</v>
+        <v>0.34309999999999974</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -1516,15 +1525,15 @@
         <v>1.8</v>
       </c>
       <c r="B70">
-        <v>-16.684899999999999</v>
+        <v>-11.771599999999999</v>
       </c>
       <c r="C70">
         <f t="shared" si="2"/>
-        <v>-16.659428571428574</v>
+        <v>-11.3924</v>
       </c>
       <c r="E70">
         <f t="shared" si="3"/>
-        <v>2.5471428571425037E-2</v>
+        <v>0.37919999999999909</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -1532,15 +1541,15 @@
         <v>1.9</v>
       </c>
       <c r="B71">
-        <v>-16.6023</v>
+        <v>-11.725899999999999</v>
       </c>
       <c r="C71">
         <f t="shared" si="2"/>
-        <v>-16.578285714285716</v>
+        <v>-11.309200000000001</v>
       </c>
       <c r="E71">
         <f t="shared" si="3"/>
-        <v>2.4014285714283545E-2</v>
+        <v>0.41669999999999874</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -1548,15 +1557,15 @@
         <v>2</v>
       </c>
       <c r="B72">
-        <v>-16.519500000000001</v>
+        <v>-11.681800000000001</v>
       </c>
       <c r="C72">
         <f t="shared" si="2"/>
-        <v>-16.497142857142858</v>
+        <v>-11.226000000000001</v>
       </c>
       <c r="E72">
         <f t="shared" si="3"/>
-        <v>2.235714285714252E-2</v>
+        <v>0.45579999999999998</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -1564,15 +1573,15 @@
         <v>2.1</v>
       </c>
       <c r="B73">
-        <v>-16.436</v>
+        <v>-11.6395</v>
       </c>
       <c r="C73">
         <f t="shared" si="2"/>
-        <v>-16.416</v>
+        <v>-11.142800000000001</v>
       </c>
       <c r="E73">
         <f t="shared" si="3"/>
-        <v>1.9999999999999574E-2</v>
+        <v>0.49669999999999881</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -1580,15 +1589,15 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B74">
-        <v>-16.352499999999999</v>
+        <v>-11.5985</v>
       </c>
       <c r="C74">
         <f t="shared" si="2"/>
-        <v>-16.334857142857143</v>
+        <v>-11.0596</v>
       </c>
       <c r="E74">
         <f t="shared" si="3"/>
-        <v>1.7642857142856627E-2</v>
+        <v>0.53889999999999993</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -1596,15 +1605,15 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B75">
-        <v>-16.268799999999999</v>
+        <v>-11.5589</v>
       </c>
       <c r="C75">
         <f t="shared" si="2"/>
-        <v>-16.253714285714288</v>
+        <v>-10.976400000000002</v>
       </c>
       <c r="E75">
         <f t="shared" si="3"/>
-        <v>1.5085714285710594E-2</v>
+        <v>0.5824999999999978</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -1612,15 +1621,15 @@
         <v>2.4</v>
       </c>
       <c r="B76">
-        <v>-16.184799999999999</v>
+        <v>-11.520899999999999</v>
       </c>
       <c r="C76">
         <f t="shared" si="2"/>
-        <v>-16.17257142857143</v>
+        <v>-10.8932</v>
       </c>
       <c r="E76">
         <f t="shared" si="3"/>
-        <v>1.2228571428568813E-2</v>
+        <v>0.62769999999999904</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -1628,15 +1637,15 @@
         <v>2.5</v>
       </c>
       <c r="B77">
-        <v>-16.1005</v>
+        <v>-11.4841</v>
       </c>
       <c r="C77">
         <f t="shared" si="2"/>
-        <v>-16.091428571428573</v>
+        <v>-10.81</v>
       </c>
       <c r="E77">
         <f t="shared" si="3"/>
-        <v>9.071428571427731E-3</v>
+        <v>0.67409999999999926</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -1644,15 +1653,15 @@
         <v>2.6</v>
       </c>
       <c r="B78">
-        <v>-16.016100000000002</v>
+        <v>-11.448600000000001</v>
       </c>
       <c r="C78">
         <f t="shared" si="2"/>
-        <v>-16.010285714285715</v>
+        <v>-10.726800000000001</v>
       </c>
       <c r="E78">
         <f t="shared" si="3"/>
-        <v>5.814285714286882E-3</v>
+        <v>0.7218</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -1660,15 +1669,15 @@
         <v>2.7</v>
       </c>
       <c r="B79">
-        <v>-15.9314</v>
+        <v>-11.414300000000001</v>
       </c>
       <c r="C79">
         <f t="shared" si="2"/>
-        <v>-15.929142857142859</v>
+        <v>-10.643600000000001</v>
       </c>
       <c r="E79">
         <f t="shared" si="3"/>
-        <v>2.2571428571414032E-3</v>
+        <v>0.77069999999999972</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -1676,271 +1685,273 @@
         <v>2.8</v>
       </c>
       <c r="B80">
-        <v>-15.846399999999999</v>
+        <v>-11.381</v>
       </c>
       <c r="C80">
         <f t="shared" si="2"/>
-        <v>-15.848000000000001</v>
+        <v>-10.560400000000001</v>
       </c>
       <c r="E80">
         <f t="shared" si="3"/>
-        <v>-1.6000000000016001E-3</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.82059999999999889</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2.9</v>
       </c>
       <c r="B81">
-        <v>-15.7613</v>
+        <v>-11.348800000000001</v>
       </c>
       <c r="C81">
         <f t="shared" si="2"/>
-        <v>-15.766857142857145</v>
+        <v>-10.4772</v>
       </c>
       <c r="E81">
         <f t="shared" si="3"/>
-        <v>-5.5571428571443704E-3</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.87160000000000082</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>3</v>
       </c>
       <c r="B82">
-        <v>-15.675800000000001</v>
+        <v>-11.317500000000001</v>
       </c>
       <c r="C82">
         <f t="shared" si="2"/>
-        <v>-15.685714285714287</v>
+        <v>-10.394</v>
       </c>
       <c r="E82">
         <f t="shared" si="3"/>
-        <v>-9.9142857142862084E-3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.92350000000000065</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>3.1</v>
       </c>
       <c r="B83">
-        <v>-15.590199999999999</v>
+        <v>-11.2872</v>
       </c>
       <c r="C83">
         <f t="shared" si="2"/>
-        <v>-15.604571428571429</v>
+        <v>-10.3108</v>
       </c>
       <c r="E83">
         <f t="shared" si="3"/>
-        <v>-1.437142857142959E-2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84">
+        <v>0.97639999999999993</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
         <v>3.2</v>
       </c>
-      <c r="B84">
-        <v>-15.504300000000001</v>
-      </c>
-      <c r="C84">
-        <f t="shared" si="2"/>
-        <v>-15.523428571428573</v>
-      </c>
-      <c r="E84">
-        <f t="shared" si="3"/>
-        <v>-1.9128571428572272E-2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B84" s="1">
+        <v>-11.2576</v>
+      </c>
+      <c r="C84" s="1">
+        <f t="shared" si="2"/>
+        <v>-10.227600000000001</v>
+      </c>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0299999999999994</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>3.3</v>
       </c>
       <c r="B85">
-        <v>-15.418200000000001</v>
+        <v>-11.228999999999999</v>
       </c>
       <c r="C85">
         <f t="shared" si="2"/>
-        <v>-15.442285714285715</v>
+        <v>-10.144400000000001</v>
       </c>
       <c r="E85">
         <f t="shared" si="3"/>
-        <v>-2.4085714285714488E-2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.0845999999999982</v>
+      </c>
+      <c r="H85" s="3"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>3.4</v>
       </c>
       <c r="B86">
-        <v>-15.332000000000001</v>
+        <v>-11.201000000000001</v>
       </c>
       <c r="C86">
         <f t="shared" si="2"/>
-        <v>-15.361142857142859</v>
+        <v>-10.061200000000001</v>
       </c>
       <c r="E86">
         <f t="shared" si="3"/>
-        <v>-2.9142857142858247E-2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.1397999999999993</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>3.5</v>
       </c>
       <c r="B87">
-        <v>-15.2455</v>
+        <v>-11.173500000000001</v>
       </c>
       <c r="C87">
         <f t="shared" si="2"/>
-        <v>-15.280000000000001</v>
+        <v>-9.9780000000000015</v>
       </c>
       <c r="E87">
         <f t="shared" si="3"/>
-        <v>-3.4500000000001307E-2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.1954999999999991</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>3.6</v>
       </c>
       <c r="B88">
-        <v>-15.158799999999999</v>
+        <v>-11.146699999999999</v>
       </c>
       <c r="C88">
         <f t="shared" si="2"/>
-        <v>-15.198857142857143</v>
+        <v>-9.8948</v>
       </c>
       <c r="E88">
         <f t="shared" si="3"/>
-        <v>-4.0057142857143901E-2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.2518999999999991</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>3.7</v>
       </c>
       <c r="B89">
-        <v>-15.071999999999999</v>
+        <v>-11.1206</v>
       </c>
       <c r="C89">
         <f t="shared" si="2"/>
-        <v>-15.117714285714287</v>
+        <v>-9.8116000000000003</v>
       </c>
       <c r="E89">
         <f t="shared" si="3"/>
-        <v>-4.5714285714288039E-2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.3089999999999993</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>3.8</v>
       </c>
       <c r="B90">
-        <v>-14.9849</v>
+        <v>-11.095000000000001</v>
       </c>
       <c r="C90">
         <f t="shared" si="2"/>
-        <v>-15.036571428571429</v>
+        <v>-9.7284000000000006</v>
       </c>
       <c r="E90">
         <f t="shared" si="3"/>
-        <v>-5.1671428571429701E-2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.3666</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>3.9</v>
       </c>
       <c r="B91">
-        <v>-14.8977</v>
+        <v>-11.07</v>
       </c>
       <c r="C91">
         <f t="shared" si="2"/>
-        <v>-14.955428571428573</v>
+        <v>-9.6452000000000009</v>
       </c>
       <c r="E91">
         <f t="shared" si="3"/>
-        <v>-5.7728571428572906E-2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.4247999999999994</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>4</v>
       </c>
       <c r="B92">
-        <v>-14.8103</v>
+        <v>-11.045500000000001</v>
       </c>
       <c r="C92">
         <f t="shared" si="2"/>
-        <v>-14.874285714285715</v>
+        <v>-9.5620000000000012</v>
       </c>
       <c r="E92">
         <f t="shared" si="3"/>
-        <v>-6.3985714285715645E-2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.4834999999999994</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>4.0999999999999996</v>
       </c>
       <c r="B93">
-        <v>-14.7227</v>
+        <v>-11.0214</v>
       </c>
       <c r="C93">
         <f t="shared" si="2"/>
-        <v>-14.793142857142858</v>
+        <v>-9.4788000000000014</v>
       </c>
       <c r="E93">
         <f t="shared" si="3"/>
-        <v>-7.0442857142857918E-2</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.5425999999999984</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>4.2</v>
       </c>
       <c r="B94">
-        <v>-14.6348</v>
+        <v>-10.9977</v>
       </c>
       <c r="C94">
         <f t="shared" si="2"/>
-        <v>-14.712000000000002</v>
+        <v>-9.3956</v>
       </c>
       <c r="E94">
         <f t="shared" si="3"/>
-        <v>-7.7200000000001268E-2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.6021000000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>4.3</v>
       </c>
       <c r="B95">
-        <v>-14.546900000000001</v>
+        <v>-10.974600000000001</v>
       </c>
       <c r="C95">
         <f t="shared" si="2"/>
-        <v>-14.630857142857144</v>
+        <v>-9.3124000000000002</v>
       </c>
       <c r="E95">
         <f t="shared" si="3"/>
-        <v>-8.3957142857142841E-2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.6622000000000003</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>4.4000000000000004</v>
       </c>
       <c r="B96">
-        <v>-14.4588</v>
+        <v>-10.9518</v>
       </c>
       <c r="C96">
         <f t="shared" si="2"/>
-        <v>-14.549714285714288</v>
+        <v>-9.2292000000000005</v>
       </c>
       <c r="E96">
         <f t="shared" si="3"/>
-        <v>-9.0914285714287502E-2</v>
+        <v>1.7225999999999999</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
@@ -1948,15 +1959,15 @@
         <v>4.5</v>
       </c>
       <c r="B97">
-        <v>-14.3706</v>
+        <v>-10.929500000000001</v>
       </c>
       <c r="C97">
         <f t="shared" si="2"/>
-        <v>-14.46857142857143</v>
+        <v>-9.1460000000000008</v>
       </c>
       <c r="E97">
         <f t="shared" si="3"/>
-        <v>-9.7971428571430152E-2</v>
+        <v>1.7835000000000001</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
@@ -1964,15 +1975,15 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="B98">
-        <v>-14.2822</v>
+        <v>-10.9076</v>
       </c>
       <c r="C98">
         <f t="shared" si="2"/>
-        <v>-14.387428571428572</v>
+        <v>-9.0628000000000011</v>
       </c>
       <c r="E98">
         <f t="shared" si="3"/>
-        <v>-0.10522857142857234</v>
+        <v>1.8447999999999993</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
@@ -1980,15 +1991,15 @@
         <v>4.7</v>
       </c>
       <c r="B99">
-        <v>-14.1936</v>
+        <v>-10.886100000000001</v>
       </c>
       <c r="C99">
         <f t="shared" si="2"/>
-        <v>-14.306285714285716</v>
+        <v>-8.9796000000000014</v>
       </c>
       <c r="E99">
         <f t="shared" si="3"/>
-        <v>-0.11268571428571583</v>
+        <v>1.9064999999999994</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
@@ -1996,15 +2007,15 @@
         <v>4.8</v>
       </c>
       <c r="B100">
-        <v>-14.105</v>
+        <v>-10.865</v>
       </c>
       <c r="C100">
         <f t="shared" si="2"/>
-        <v>-14.225142857142858</v>
+        <v>-8.8963999999999999</v>
       </c>
       <c r="E100">
         <f t="shared" si="3"/>
-        <v>-0.12014285714285755</v>
+        <v>1.9686000000000003</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
@@ -2012,15 +2023,15 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="B101">
-        <v>-14.0162</v>
+        <v>-10.8443</v>
       </c>
       <c r="C101">
         <f t="shared" si="2"/>
-        <v>-14.144000000000002</v>
+        <v>-8.8132000000000001</v>
       </c>
       <c r="E101">
         <f t="shared" si="3"/>
-        <v>-0.12780000000000236</v>
+        <v>2.0311000000000003</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
@@ -2028,15 +2039,15 @@
         <v>5</v>
       </c>
       <c r="B102">
-        <v>-13.927199999999999</v>
+        <v>-10.824</v>
       </c>
       <c r="C102">
         <f t="shared" si="2"/>
-        <v>-14.062857142857144</v>
+        <v>-8.73</v>
       </c>
       <c r="E102">
         <f t="shared" si="3"/>
-        <v>-0.13565714285714492</v>
+        <v>2.0939999999999994</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
@@ -2044,15 +2055,15 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B103">
-        <v>-13.838200000000001</v>
+        <v>-10.804</v>
       </c>
       <c r="C103">
         <f t="shared" si="2"/>
-        <v>-13.981714285714286</v>
+        <v>-8.6468000000000007</v>
       </c>
       <c r="E103">
         <f t="shared" si="3"/>
-        <v>-0.14351428571428571</v>
+        <v>2.1571999999999996</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
@@ -2060,15 +2071,15 @@
         <v>5.2</v>
       </c>
       <c r="B104">
-        <v>-13.749000000000001</v>
+        <v>-10.7845</v>
       </c>
       <c r="C104">
         <f t="shared" si="2"/>
-        <v>-13.900571428571428</v>
+        <v>-8.563600000000001</v>
       </c>
       <c r="E104">
         <f t="shared" si="3"/>
-        <v>-0.1515714285714278</v>
+        <v>2.2208999999999985</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
@@ -2076,15 +2087,15 @@
         <v>5.3</v>
       </c>
       <c r="B105">
-        <v>-13.659800000000001</v>
+        <v>-10.7654</v>
       </c>
       <c r="C105">
         <f t="shared" si="2"/>
-        <v>-13.819428571428574</v>
+        <v>-8.4804000000000013</v>
       </c>
       <c r="E105">
         <f t="shared" si="3"/>
-        <v>-0.15962857142857345</v>
+        <v>2.2849999999999984</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
@@ -2092,15 +2103,15 @@
         <v>5.4</v>
       </c>
       <c r="B106">
-        <v>-13.570399999999999</v>
+        <v>-10.746600000000001</v>
       </c>
       <c r="C106">
         <f t="shared" si="2"/>
-        <v>-13.738285714285716</v>
+        <v>-8.3972000000000016</v>
       </c>
       <c r="E106">
         <f t="shared" si="3"/>
-        <v>-0.16788571428571686</v>
+        <v>2.3493999999999993</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
@@ -2108,15 +2119,15 @@
         <v>5.5</v>
       </c>
       <c r="B107">
-        <v>-13.4809</v>
+        <v>-10.728300000000001</v>
       </c>
       <c r="C107">
         <f t="shared" si="2"/>
-        <v>-13.657142857142858</v>
+        <v>-8.3140000000000001</v>
       </c>
       <c r="E107">
         <f t="shared" si="3"/>
-        <v>-0.17624285714285826</v>
+        <v>2.4143000000000008</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -2124,15 +2135,15 @@
         <v>5.6</v>
       </c>
       <c r="B108">
-        <v>-13.391400000000001</v>
+        <v>-10.7104</v>
       </c>
       <c r="C108">
         <f t="shared" si="2"/>
-        <v>-13.576000000000001</v>
+        <v>-8.2308000000000021</v>
       </c>
       <c r="E108">
         <f t="shared" si="3"/>
-        <v>-0.18459999999999965</v>
+        <v>2.4795999999999978</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
@@ -2140,15 +2151,15 @@
         <v>5.7</v>
       </c>
       <c r="B109">
-        <v>-13.3017</v>
+        <v>-10.6929</v>
       </c>
       <c r="C109">
         <f t="shared" si="2"/>
-        <v>-13.494857142857143</v>
+        <v>-8.1476000000000006</v>
       </c>
       <c r="E109">
         <f t="shared" si="3"/>
-        <v>-0.19315714285714236</v>
+        <v>2.5452999999999992</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
@@ -2156,15 +2167,15 @@
         <v>5.8</v>
       </c>
       <c r="B110">
-        <v>-13.212</v>
+        <v>-10.675800000000001</v>
       </c>
       <c r="C110">
         <f t="shared" si="2"/>
-        <v>-13.413714285714288</v>
+        <v>-8.0644000000000009</v>
       </c>
       <c r="E110">
         <f t="shared" si="3"/>
-        <v>-0.20171428571428862</v>
+        <v>2.6113999999999997</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
@@ -2172,15 +2183,15 @@
         <v>5.9</v>
       </c>
       <c r="B111">
-        <v>-13.122199999999999</v>
+        <v>-10.6591</v>
       </c>
       <c r="C111">
         <f t="shared" si="2"/>
-        <v>-13.332571428571431</v>
+        <v>-7.9812000000000003</v>
       </c>
       <c r="E111">
         <f t="shared" si="3"/>
-        <v>-0.2103714285714311</v>
+        <v>2.6779000000000002</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
@@ -2188,15 +2199,15 @@
         <v>6</v>
       </c>
       <c r="B112">
-        <v>-13.032400000000001</v>
+        <v>-10.642899999999999</v>
       </c>
       <c r="C112">
         <f t="shared" si="2"/>
-        <v>-13.251428571428573</v>
+        <v>-7.8980000000000006</v>
       </c>
       <c r="E112">
         <f t="shared" si="3"/>
-        <v>-0.21902857142857179</v>
+        <v>2.7448999999999986</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
@@ -2204,15 +2215,15 @@
         <v>6.1</v>
       </c>
       <c r="B113">
-        <v>-12.942500000000001</v>
+        <v>-10.6271</v>
       </c>
       <c r="C113">
         <f t="shared" si="2"/>
-        <v>-13.170285714285715</v>
+        <v>-7.8148000000000009</v>
       </c>
       <c r="E113">
         <f t="shared" si="3"/>
-        <v>-0.22778571428571404</v>
+        <v>2.8122999999999996</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
@@ -2220,15 +2231,15 @@
         <v>6.2</v>
       </c>
       <c r="B114">
-        <v>-12.852600000000001</v>
+        <v>-10.611700000000001</v>
       </c>
       <c r="C114">
         <f t="shared" si="2"/>
-        <v>-13.089142857142857</v>
+        <v>-7.7316000000000003</v>
       </c>
       <c r="E114">
         <f t="shared" si="3"/>
-        <v>-0.23654285714285628</v>
+        <v>2.8801000000000005</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -2236,15 +2247,15 @@
         <v>6.3</v>
       </c>
       <c r="B115">
-        <v>-12.762600000000001</v>
+        <v>-10.5968</v>
       </c>
       <c r="C115">
         <f t="shared" si="2"/>
-        <v>-13.008000000000003</v>
+        <v>-7.6484000000000005</v>
       </c>
       <c r="E115">
         <f t="shared" si="3"/>
-        <v>-0.24540000000000184</v>
+        <v>2.9483999999999995</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -2252,15 +2263,15 @@
         <v>6.4</v>
       </c>
       <c r="B116">
-        <v>-12.672599999999999</v>
+        <v>-10.5822</v>
       </c>
       <c r="C116">
         <f t="shared" si="2"/>
-        <v>-12.926857142857145</v>
+        <v>-7.5652000000000008</v>
       </c>
       <c r="E116">
         <f t="shared" si="3"/>
-        <v>-0.25425714285714562</v>
+        <v>3.0169999999999995</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -2268,15 +2279,15 @@
         <v>6.5</v>
       </c>
       <c r="B117">
-        <v>-12.582599999999999</v>
+        <v>-10.568099999999999</v>
       </c>
       <c r="C117">
         <f t="shared" si="2"/>
-        <v>-12.845714285714287</v>
+        <v>-7.4820000000000011</v>
       </c>
       <c r="E117">
         <f t="shared" si="3"/>
-        <v>-0.26311428571428763</v>
+        <v>3.0860999999999983</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
@@ -2284,15 +2295,15 @@
         <v>6.6</v>
       </c>
       <c r="B118">
-        <v>-12.492599999999999</v>
+        <v>-10.554500000000001</v>
       </c>
       <c r="C118">
         <f t="shared" si="2"/>
-        <v>-12.764571428571429</v>
+        <v>-7.3988000000000014</v>
       </c>
       <c r="E118">
         <f t="shared" si="3"/>
-        <v>-0.27197142857142964</v>
+        <v>3.1556999999999995</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
@@ -2300,15 +2311,15 @@
         <v>6.7</v>
       </c>
       <c r="B119">
-        <v>-12.402699999999999</v>
+        <v>-10.5412</v>
       </c>
       <c r="C119">
         <f t="shared" si="2"/>
-        <v>-12.683428571428571</v>
+        <v>-7.3156000000000008</v>
       </c>
       <c r="E119">
         <f t="shared" si="3"/>
-        <v>-0.28072857142857188</v>
+        <v>3.2255999999999991</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
@@ -2316,15 +2327,15 @@
         <v>6.8</v>
       </c>
       <c r="B120">
-        <v>-12.3127</v>
+        <v>-10.5284</v>
       </c>
       <c r="C120">
         <f t="shared" si="2"/>
-        <v>-12.602285714285717</v>
+        <v>-7.2324000000000011</v>
       </c>
       <c r="E120">
         <f t="shared" si="3"/>
-        <v>-0.28958571428571744</v>
+        <v>3.2959999999999985</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
@@ -2332,15 +2343,15 @@
         <v>6.9</v>
       </c>
       <c r="B121">
-        <v>-12.222799999999999</v>
+        <v>-10.5159</v>
       </c>
       <c r="C121">
         <f t="shared" si="2"/>
-        <v>-12.521142857142859</v>
+        <v>-7.1492000000000004</v>
       </c>
       <c r="E121">
         <f t="shared" si="3"/>
-        <v>-0.29834285714285969</v>
+        <v>3.3666999999999998</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
@@ -2348,15 +2359,15 @@
         <v>7</v>
       </c>
       <c r="B122">
-        <v>-12.132999999999999</v>
+        <v>-10.5039</v>
       </c>
       <c r="C122">
         <f t="shared" si="2"/>
-        <v>-12.440000000000001</v>
+        <v>-7.0660000000000007</v>
       </c>
       <c r="E122">
         <f t="shared" si="3"/>
-        <v>-0.30700000000000216</v>
+        <v>3.4378999999999991</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
@@ -2364,15 +2375,15 @@
         <v>7.1</v>
       </c>
       <c r="B123">
-        <v>-12.0433</v>
+        <v>-10.4922</v>
       </c>
       <c r="C123">
         <f t="shared" si="2"/>
-        <v>-12.358857142857143</v>
+        <v>-6.982800000000001</v>
       </c>
       <c r="E123">
         <f t="shared" si="3"/>
-        <v>-0.31555714285714309</v>
+        <v>3.5093999999999994</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
@@ -2380,15 +2391,15 @@
         <v>7.2</v>
       </c>
       <c r="B124">
-        <v>-11.9537</v>
+        <v>-10.4809</v>
       </c>
       <c r="C124">
         <f t="shared" si="2"/>
-        <v>-12.277714285714286</v>
+        <v>-6.8996000000000004</v>
       </c>
       <c r="E124">
         <f t="shared" si="3"/>
-        <v>-0.32401428571428603</v>
+        <v>3.5812999999999997</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -2396,15 +2407,15 @@
         <v>7.3</v>
       </c>
       <c r="B125">
-        <v>-11.8642</v>
+        <v>-10.47</v>
       </c>
       <c r="C125">
         <f t="shared" si="2"/>
-        <v>-12.196571428571431</v>
+        <v>-6.8164000000000007</v>
       </c>
       <c r="E125">
         <f t="shared" si="3"/>
-        <v>-0.33237142857143098</v>
+        <v>3.6536</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
@@ -2412,15 +2423,15 @@
         <v>7.4</v>
       </c>
       <c r="B126">
-        <v>-11.774900000000001</v>
+        <v>-10.4594</v>
       </c>
       <c r="C126">
         <f t="shared" si="2"/>
-        <v>-12.115428571428573</v>
+        <v>-6.733200000000001</v>
       </c>
       <c r="E126">
         <f t="shared" si="3"/>
-        <v>-0.34052857142857285</v>
+        <v>3.7261999999999995</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
@@ -2428,15 +2439,15 @@
         <v>7.5</v>
       </c>
       <c r="B127">
-        <v>-11.685700000000001</v>
+        <v>-10.449199999999999</v>
       </c>
       <c r="C127">
         <f t="shared" si="2"/>
-        <v>-12.034285714285716</v>
+        <v>-6.6500000000000012</v>
       </c>
       <c r="E127">
         <f t="shared" si="3"/>
-        <v>-0.34858571428571494</v>
+        <v>3.7991999999999981</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
@@ -2444,15 +2455,15 @@
         <v>7.6</v>
       </c>
       <c r="B128">
-        <v>-11.5968</v>
+        <v>-10.439299999999999</v>
       </c>
       <c r="C128">
         <f t="shared" si="2"/>
-        <v>-11.953142857142858</v>
+        <v>-6.5668000000000015</v>
       </c>
       <c r="E128">
         <f t="shared" si="3"/>
-        <v>-0.35634285714285774</v>
+        <v>3.8724999999999978</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -2460,15 +2471,15 @@
         <v>7.7</v>
       </c>
       <c r="B129">
-        <v>-11.5082</v>
+        <v>-10.4297</v>
       </c>
       <c r="C129">
         <f t="shared" si="2"/>
-        <v>-11.872</v>
+        <v>-6.4836000000000009</v>
       </c>
       <c r="E129">
         <f t="shared" si="3"/>
-        <v>-0.36379999999999946</v>
+        <v>3.9460999999999995</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -2476,15 +2487,15 @@
         <v>7.8</v>
       </c>
       <c r="B130">
-        <v>-11.4199</v>
+        <v>-10.420400000000001</v>
       </c>
       <c r="C130">
         <f t="shared" si="2"/>
-        <v>-11.790857142857146</v>
+        <v>-6.4004000000000012</v>
       </c>
       <c r="E130">
         <f t="shared" si="3"/>
-        <v>-0.37095714285714543</v>
+        <v>4.0199999999999996</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -2492,15 +2503,15 @@
         <v>7.9</v>
       </c>
       <c r="B131">
-        <v>-11.332000000000001</v>
+        <v>-10.4114</v>
       </c>
       <c r="C131">
-        <f t="shared" ref="C131:C194" si="4">((142/175)*A131) -18.12</f>
-        <v>-11.709714285714288</v>
+        <f t="shared" ref="C131:C194" si="4">((104/125)*A131) -12.89</f>
+        <v>-6.3172000000000006</v>
       </c>
       <c r="E131">
         <f t="shared" ref="E131:E194" si="5">C131-B131</f>
-        <v>-0.377714285714287</v>
+        <v>4.0941999999999998</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -2508,15 +2519,15 @@
         <v>8</v>
       </c>
       <c r="B132">
-        <v>-11.2445</v>
+        <v>-10.402699999999999</v>
       </c>
       <c r="C132">
         <f t="shared" si="4"/>
-        <v>-11.62857142857143</v>
+        <v>-6.2340000000000009</v>
       </c>
       <c r="E132">
         <f t="shared" si="5"/>
-        <v>-0.38407142857142951</v>
+        <v>4.1686999999999985</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -2524,15 +2535,15 @@
         <v>8.1</v>
       </c>
       <c r="B133">
-        <v>-11.157500000000001</v>
+        <v>-10.394299999999999</v>
       </c>
       <c r="C133">
         <f t="shared" si="4"/>
-        <v>-11.547428571428572</v>
+        <v>-6.1508000000000012</v>
       </c>
       <c r="E133">
         <f t="shared" si="5"/>
-        <v>-0.3899285714285714</v>
+        <v>4.2434999999999983</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -2540,15 +2551,15 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B134">
-        <v>-11.071099999999999</v>
+        <v>-10.386100000000001</v>
       </c>
       <c r="C134">
         <f t="shared" si="4"/>
-        <v>-11.466285714285716</v>
+        <v>-6.0676000000000014</v>
       </c>
       <c r="E134">
         <f t="shared" si="5"/>
-        <v>-0.39518571428571647</v>
+        <v>4.3184999999999993</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -2556,15 +2567,15 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="B135">
-        <v>-10.985300000000001</v>
+        <v>-10.3782</v>
       </c>
       <c r="C135">
         <f t="shared" si="4"/>
-        <v>-11.385142857142858</v>
+        <v>-5.9843999999999999</v>
       </c>
       <c r="E135">
         <f t="shared" si="5"/>
-        <v>-0.39984285714285761</v>
+        <v>4.3937999999999997</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -2572,15 +2583,15 @@
         <v>8.4</v>
       </c>
       <c r="B136">
-        <v>-10.9003</v>
+        <v>-10.3706</v>
       </c>
       <c r="C136">
         <f t="shared" si="4"/>
-        <v>-11.304000000000002</v>
+        <v>-5.9012000000000002</v>
       </c>
       <c r="E136">
         <f t="shared" si="5"/>
-        <v>-0.40370000000000239</v>
+        <v>4.4693999999999994</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -2588,15 +2599,15 @@
         <v>8.5</v>
       </c>
       <c r="B137">
-        <v>-10.8161</v>
+        <v>-10.363200000000001</v>
       </c>
       <c r="C137">
         <f t="shared" si="4"/>
-        <v>-11.222857142857144</v>
+        <v>-5.8180000000000005</v>
       </c>
       <c r="E137">
         <f t="shared" si="5"/>
-        <v>-0.40675714285714371</v>
+        <v>4.5452000000000004</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
@@ -2604,15 +2615,15 @@
         <v>8.6</v>
       </c>
       <c r="B138">
-        <v>-10.732799999999999</v>
+        <v>-10.356</v>
       </c>
       <c r="C138">
         <f t="shared" si="4"/>
-        <v>-11.141714285714286</v>
+        <v>-5.7348000000000008</v>
       </c>
       <c r="E138">
         <f t="shared" si="5"/>
-        <v>-0.40891428571428712</v>
+        <v>4.6211999999999991</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -2620,15 +2631,15 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="B139">
-        <v>-10.650600000000001</v>
+        <v>-10.349</v>
       </c>
       <c r="C139">
         <f t="shared" si="4"/>
-        <v>-11.06057142857143</v>
+        <v>-5.6516000000000011</v>
       </c>
       <c r="E139">
         <f t="shared" si="5"/>
-        <v>-0.40997142857142954</v>
+        <v>4.6973999999999991</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
@@ -2636,15 +2647,15 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="B140">
-        <v>-10.569699999999999</v>
+        <v>-10.3423</v>
       </c>
       <c r="C140">
         <f t="shared" si="4"/>
-        <v>-10.979428571428572</v>
+        <v>-5.5684000000000005</v>
       </c>
       <c r="E140">
         <f t="shared" si="5"/>
-        <v>-0.40972857142857322</v>
+        <v>4.7738999999999994</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
@@ -2652,15 +2663,15 @@
         <v>8.9</v>
       </c>
       <c r="B141">
-        <v>-10.49</v>
+        <v>-10.335800000000001</v>
       </c>
       <c r="C141">
         <f t="shared" si="4"/>
-        <v>-10.898285714285716</v>
+        <v>-5.4852000000000007</v>
       </c>
       <c r="E141">
         <f t="shared" si="5"/>
-        <v>-0.40828571428571614</v>
+        <v>4.8506</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
@@ -2668,15 +2679,15 @@
         <v>9</v>
       </c>
       <c r="B142">
-        <v>-10.4117</v>
+        <v>-10.3294</v>
       </c>
       <c r="C142">
         <f t="shared" si="4"/>
-        <v>-10.817142857142859</v>
+        <v>-5.402000000000001</v>
       </c>
       <c r="E142">
         <f t="shared" si="5"/>
-        <v>-0.40544285714285877</v>
+        <v>4.9273999999999987</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
@@ -2684,15 +2695,15 @@
         <v>9.1</v>
       </c>
       <c r="B143">
-        <v>-10.335100000000001</v>
+        <v>-10.3233</v>
       </c>
       <c r="C143">
         <f t="shared" si="4"/>
-        <v>-10.736000000000001</v>
+        <v>-5.3188000000000013</v>
       </c>
       <c r="E143">
         <f t="shared" si="5"/>
-        <v>-0.40090000000000003</v>
+        <v>5.0044999999999984</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
@@ -2700,15 +2711,15 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B144">
-        <v>-10.26</v>
+        <v>-10.317399999999999</v>
       </c>
       <c r="C144">
         <f t="shared" si="4"/>
-        <v>-10.654857142857145</v>
+        <v>-5.2356000000000016</v>
       </c>
       <c r="E144">
         <f t="shared" si="5"/>
-        <v>-0.39485714285714479</v>
+        <v>5.0817999999999977</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
@@ -2716,15 +2727,15 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="B145">
-        <v>-10.1867</v>
+        <v>-10.3116</v>
       </c>
       <c r="C145">
         <f t="shared" si="4"/>
-        <v>-10.573714285714287</v>
+        <v>-5.1524000000000001</v>
       </c>
       <c r="E145">
         <f t="shared" si="5"/>
-        <v>-0.38701428571428664</v>
+        <v>5.1592000000000002</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
@@ -2732,15 +2743,15 @@
         <v>9.4</v>
       </c>
       <c r="B146">
-        <v>-10.1151</v>
+        <v>-10.305999999999999</v>
       </c>
       <c r="C146">
         <f t="shared" si="4"/>
-        <v>-10.492571428571431</v>
+        <v>-5.0692000000000004</v>
       </c>
       <c r="E146">
         <f t="shared" si="5"/>
-        <v>-0.37747142857143068</v>
+        <v>5.2367999999999988</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
@@ -2748,15 +2759,15 @@
         <v>9.5</v>
       </c>
       <c r="B147">
-        <v>-10.045299999999999</v>
+        <v>-10.300599999999999</v>
       </c>
       <c r="C147">
         <f t="shared" si="4"/>
-        <v>-10.411428571428573</v>
+        <v>-4.9860000000000007</v>
       </c>
       <c r="E147">
         <f t="shared" si="5"/>
-        <v>-0.36612857142857358</v>
+        <v>5.3145999999999987</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
@@ -2764,15 +2775,15 @@
         <v>9.6</v>
       </c>
       <c r="B148">
-        <v>-9.9774899999999995</v>
+        <v>-10.295400000000001</v>
       </c>
       <c r="C148">
         <f t="shared" si="4"/>
-        <v>-10.330285714285715</v>
+        <v>-4.9028000000000009</v>
       </c>
       <c r="E148">
         <f t="shared" si="5"/>
-        <v>-0.35279571428571543</v>
+        <v>5.3925999999999998</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
@@ -2780,15 +2791,15 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="B149">
-        <v>-9.9114299999999993</v>
+        <v>-10.2903</v>
       </c>
       <c r="C149">
         <f t="shared" si="4"/>
-        <v>-10.249142857142859</v>
+        <v>-4.8196000000000012</v>
       </c>
       <c r="E149">
         <f t="shared" si="5"/>
-        <v>-0.33771285714285959</v>
+        <v>5.470699999999999</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
@@ -2796,15 +2807,15 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="B150">
-        <v>-9.8470099999999992</v>
+        <v>-10.285399999999999</v>
       </c>
       <c r="C150">
         <f t="shared" si="4"/>
-        <v>-10.168000000000001</v>
+        <v>-4.7363999999999997</v>
       </c>
       <c r="E150">
         <f t="shared" si="5"/>
-        <v>-0.32099000000000188</v>
+        <v>5.5489999999999995</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
@@ -2812,15 +2823,15 @@
         <v>9.9</v>
       </c>
       <c r="B151">
-        <v>-9.7848900000000008</v>
+        <v>-10.2806</v>
       </c>
       <c r="C151">
         <f t="shared" si="4"/>
-        <v>-10.086857142857143</v>
+        <v>-4.6532</v>
       </c>
       <c r="E151">
         <f t="shared" si="5"/>
-        <v>-0.30196714285714243</v>
+        <v>5.6273999999999997</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
@@ -2828,15 +2839,15 @@
         <v>10</v>
       </c>
       <c r="B152">
-        <v>-9.7243200000000005</v>
+        <v>-10.2759</v>
       </c>
       <c r="C152">
         <f t="shared" si="4"/>
-        <v>-10.005714285714287</v>
+        <v>-4.57</v>
       </c>
       <c r="E152">
         <f t="shared" si="5"/>
-        <v>-0.2813942857142866</v>
+        <v>5.7058999999999997</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -2844,15 +2855,15 @@
         <v>10.1</v>
       </c>
       <c r="B153">
-        <v>-9.6656999999999993</v>
+        <v>-10.2714</v>
       </c>
       <c r="C153">
         <f t="shared" si="4"/>
-        <v>-9.924571428571431</v>
+        <v>-4.4868000000000006</v>
       </c>
       <c r="E153">
         <f t="shared" si="5"/>
-        <v>-0.25887142857143175</v>
+        <v>5.7845999999999993</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
@@ -2860,15 +2871,15 @@
         <v>10.199999999999999</v>
       </c>
       <c r="B154">
-        <v>-9.6087799999999994</v>
+        <v>-10.266999999999999</v>
       </c>
       <c r="C154">
         <f t="shared" si="4"/>
-        <v>-9.8434285714285732</v>
+        <v>-4.4036000000000008</v>
       </c>
       <c r="E154">
         <f t="shared" si="5"/>
-        <v>-0.23464857142857376</v>
+        <v>5.8633999999999986</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -2876,15 +2887,15 @@
         <v>10.3</v>
       </c>
       <c r="B155">
-        <v>-9.5535499999999995</v>
+        <v>-10.262700000000001</v>
       </c>
       <c r="C155">
         <f t="shared" si="4"/>
-        <v>-9.7622857142857153</v>
+        <v>-4.3204000000000011</v>
       </c>
       <c r="E155">
         <f t="shared" si="5"/>
-        <v>-0.2087357142857158</v>
+        <v>5.9422999999999995</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -2892,15 +2903,15 @@
         <v>10.4</v>
       </c>
       <c r="B156">
-        <v>-9.5002999999999993</v>
+        <v>-10.258599999999999</v>
       </c>
       <c r="C156">
         <f t="shared" si="4"/>
-        <v>-9.6811428571428575</v>
+        <v>-4.2372000000000014</v>
       </c>
       <c r="E156">
         <f t="shared" si="5"/>
-        <v>-0.18084285714285819</v>
+        <v>6.0213999999999981</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -2908,15 +2919,15 @@
         <v>10.5</v>
       </c>
       <c r="B157">
-        <v>-9.4486699999999999</v>
+        <v>-10.2545</v>
       </c>
       <c r="C157">
         <f t="shared" si="4"/>
-        <v>-9.6000000000000014</v>
+        <v>-4.1540000000000017</v>
       </c>
       <c r="E157">
         <f t="shared" si="5"/>
-        <v>-0.15133000000000152</v>
+        <v>6.1004999999999985</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
@@ -2924,15 +2935,15 @@
         <v>10.6</v>
       </c>
       <c r="B158">
-        <v>-9.3987599999999993</v>
+        <v>-10.2506</v>
       </c>
       <c r="C158">
         <f t="shared" si="4"/>
-        <v>-9.5188571428571453</v>
+        <v>-4.070800000000002</v>
       </c>
       <c r="E158">
         <f t="shared" si="5"/>
-        <v>-0.12009714285714601</v>
+        <v>6.1797999999999984</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
@@ -2940,15 +2951,15 @@
         <v>10.7</v>
       </c>
       <c r="B159">
-        <v>-9.3505500000000001</v>
+        <v>-10.246700000000001</v>
       </c>
       <c r="C159">
         <f t="shared" si="4"/>
-        <v>-9.4377142857142875</v>
+        <v>-3.9876000000000023</v>
       </c>
       <c r="E159">
         <f t="shared" si="5"/>
-        <v>-8.7164285714287359E-2</v>
+        <v>6.2590999999999983</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
@@ -2956,15 +2967,15 @@
         <v>10.8</v>
       </c>
       <c r="B160">
-        <v>-9.3039900000000006</v>
+        <v>-10.243</v>
       </c>
       <c r="C160">
         <f t="shared" si="4"/>
-        <v>-9.3565714285714296</v>
+        <v>-3.9044000000000008</v>
       </c>
       <c r="E160">
         <f t="shared" si="5"/>
-        <v>-5.2581428571429001E-2</v>
+        <v>6.3385999999999996</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
@@ -2972,15 +2983,15 @@
         <v>10.9</v>
       </c>
       <c r="B161">
-        <v>-9.2590599999999998</v>
+        <v>-10.2393</v>
       </c>
       <c r="C161">
         <f t="shared" si="4"/>
-        <v>-9.2754285714285718</v>
+        <v>-3.821200000000001</v>
       </c>
       <c r="E161">
         <f t="shared" si="5"/>
-        <v>-1.6368571428571954E-2</v>
+        <v>6.418099999999999</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
@@ -2988,15 +2999,15 @@
         <v>11</v>
       </c>
       <c r="B162">
-        <v>-9.2157099999999996</v>
+        <v>-10.2357</v>
       </c>
       <c r="C162">
         <f t="shared" si="4"/>
-        <v>-9.1942857142857157</v>
+        <v>-3.7380000000000013</v>
       </c>
       <c r="E162">
         <f t="shared" si="5"/>
-        <v>2.1424285714283897E-2</v>
+        <v>6.4976999999999983</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
@@ -3004,15 +3015,15 @@
         <v>11.1</v>
       </c>
       <c r="B163">
-        <v>-9.1738800000000005</v>
+        <v>-10.2323</v>
       </c>
       <c r="C163">
         <f t="shared" si="4"/>
-        <v>-9.1131428571428597</v>
+        <v>-3.6548000000000016</v>
       </c>
       <c r="E163">
         <f t="shared" si="5"/>
-        <v>6.0737142857140825E-2</v>
+        <v>6.5774999999999988</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
@@ -3020,15 +3031,15 @@
         <v>11.2</v>
       </c>
       <c r="B164">
-        <v>-9.1335200000000007</v>
+        <v>-10.2288</v>
       </c>
       <c r="C164">
         <f t="shared" si="4"/>
-        <v>-9.0320000000000018</v>
+        <v>-3.5716000000000019</v>
       </c>
       <c r="E164">
         <f t="shared" si="5"/>
-        <v>0.10151999999999894</v>
+        <v>6.6571999999999978</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
@@ -3036,15 +3047,15 @@
         <v>11.3</v>
       </c>
       <c r="B165">
-        <v>-9.0945599999999995</v>
+        <v>-10.2255</v>
       </c>
       <c r="C165">
         <f t="shared" si="4"/>
-        <v>-8.950857142857144</v>
+        <v>-3.4884000000000004</v>
       </c>
       <c r="E165">
         <f t="shared" si="5"/>
-        <v>0.14370285714285558</v>
+        <v>6.7370999999999999</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
@@ -3052,15 +3063,15 @@
         <v>11.4</v>
       </c>
       <c r="B166">
-        <v>-9.0569400000000009</v>
+        <v>-10.222200000000001</v>
       </c>
       <c r="C166">
         <f t="shared" si="4"/>
-        <v>-8.8697142857142861</v>
+        <v>-3.4052000000000007</v>
       </c>
       <c r="E166">
         <f t="shared" si="5"/>
-        <v>0.18722571428571477</v>
+        <v>6.8170000000000002</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
@@ -3068,15 +3079,15 @@
         <v>11.5</v>
       </c>
       <c r="B167">
-        <v>-9.0205800000000007</v>
+        <v>-10.218999999999999</v>
       </c>
       <c r="C167">
         <f t="shared" si="4"/>
-        <v>-8.78857142857143</v>
+        <v>-3.322000000000001</v>
       </c>
       <c r="E167">
         <f t="shared" si="5"/>
-        <v>0.23200857142857068</v>
+        <v>6.8969999999999985</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
@@ -3084,15 +3095,15 @@
         <v>11.6</v>
       </c>
       <c r="B168">
-        <v>-8.9854099999999999</v>
+        <v>-10.2159</v>
       </c>
       <c r="C168">
         <f t="shared" si="4"/>
-        <v>-8.707428571428574</v>
+        <v>-3.2388000000000012</v>
       </c>
       <c r="E168">
         <f t="shared" si="5"/>
-        <v>0.27798142857142594</v>
+        <v>6.9770999999999983</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
@@ -3100,15 +3111,15 @@
         <v>11.7</v>
       </c>
       <c r="B169">
-        <v>-8.9513599999999993</v>
+        <v>-10.2128</v>
       </c>
       <c r="C169">
         <f t="shared" si="4"/>
-        <v>-8.6262857142857161</v>
+        <v>-3.1556000000000015</v>
       </c>
       <c r="E169">
         <f t="shared" si="5"/>
-        <v>0.32507428571428321</v>
+        <v>7.0571999999999981</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
@@ -3116,15 +3127,15 @@
         <v>11.8</v>
       </c>
       <c r="B170">
-        <v>-8.9183599999999998</v>
+        <v>-10.2098</v>
       </c>
       <c r="C170">
         <f t="shared" si="4"/>
-        <v>-8.5451428571428583</v>
+        <v>-3.0724</v>
       </c>
       <c r="E170">
         <f t="shared" si="5"/>
-        <v>0.37321714285714158</v>
+        <v>7.1373999999999995</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
@@ -3132,15 +3143,15 @@
         <v>11.9</v>
       </c>
       <c r="B171">
-        <v>-8.8863299999999992</v>
+        <v>-10.206799999999999</v>
       </c>
       <c r="C171">
         <f t="shared" si="4"/>
-        <v>-8.4640000000000004</v>
+        <v>-2.9892000000000003</v>
       </c>
       <c r="E171">
         <f t="shared" si="5"/>
-        <v>0.42232999999999876</v>
+        <v>7.2175999999999991</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
@@ -3148,15 +3159,15 @@
         <v>12</v>
       </c>
       <c r="B172">
-        <v>-8.8552199999999992</v>
+        <v>-10.203900000000001</v>
       </c>
       <c r="C172">
         <f t="shared" si="4"/>
-        <v>-8.3828571428571443</v>
+        <v>-2.9060000000000006</v>
       </c>
       <c r="E172">
         <f t="shared" si="5"/>
-        <v>0.47236285714285486</v>
+        <v>7.2979000000000003</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
@@ -3164,15 +3175,15 @@
         <v>12.1</v>
       </c>
       <c r="B173">
-        <v>-8.8249600000000008</v>
+        <v>-10.201000000000001</v>
       </c>
       <c r="C173">
         <f t="shared" si="4"/>
-        <v>-8.3017142857142883</v>
+        <v>-2.8228000000000009</v>
       </c>
       <c r="E173">
         <f t="shared" si="5"/>
-        <v>0.52324571428571254</v>
+        <v>7.3781999999999996</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
@@ -3180,15 +3191,15 @@
         <v>12.2</v>
       </c>
       <c r="B174">
-        <v>-8.7954899999999991</v>
+        <v>-10.1982</v>
       </c>
       <c r="C174">
         <f t="shared" si="4"/>
-        <v>-8.2205714285714304</v>
+        <v>-2.7396000000000011</v>
       </c>
       <c r="E174">
         <f t="shared" si="5"/>
-        <v>0.57491857142856873</v>
+        <v>7.4585999999999988</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
@@ -3196,15 +3207,15 @@
         <v>12.3</v>
       </c>
       <c r="B175">
-        <v>-8.76675</v>
+        <v>-10.195399999999999</v>
       </c>
       <c r="C175">
         <f t="shared" si="4"/>
-        <v>-8.1394285714285726</v>
+        <v>-2.6563999999999997</v>
       </c>
       <c r="E175">
         <f t="shared" si="5"/>
-        <v>0.62732142857142748</v>
+        <v>7.5389999999999997</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
@@ -3212,15 +3223,15 @@
         <v>12.4</v>
       </c>
       <c r="B176">
-        <v>-8.7386999999999997</v>
+        <v>-10.192600000000001</v>
       </c>
       <c r="C176">
         <f t="shared" si="4"/>
-        <v>-8.0582857142857147</v>
+        <v>-2.5731999999999999</v>
       </c>
       <c r="E176">
         <f t="shared" si="5"/>
-        <v>0.68041428571428497</v>
+        <v>7.6194000000000006</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
@@ -3228,15 +3239,15 @@
         <v>12.5</v>
       </c>
       <c r="B177">
-        <v>-8.7112800000000004</v>
+        <v>-10.1899</v>
       </c>
       <c r="C177">
         <f t="shared" si="4"/>
-        <v>-7.9771428571428586</v>
+        <v>-2.4900000000000002</v>
       </c>
       <c r="E177">
         <f t="shared" si="5"/>
-        <v>0.73413714285714171</v>
+        <v>7.6998999999999995</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
@@ -3244,15 +3255,15 @@
         <v>12.6</v>
       </c>
       <c r="B178">
-        <v>-8.6844599999999996</v>
+        <v>-10.1873</v>
       </c>
       <c r="C178">
         <f t="shared" si="4"/>
-        <v>-7.8960000000000026</v>
+        <v>-2.4068000000000005</v>
       </c>
       <c r="E178">
         <f t="shared" si="5"/>
-        <v>0.78845999999999705</v>
+        <v>7.7805</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
@@ -3260,15 +3271,15 @@
         <v>12.7</v>
       </c>
       <c r="B179">
-        <v>-8.6582000000000008</v>
+        <v>-10.1846</v>
       </c>
       <c r="C179">
         <f t="shared" si="4"/>
-        <v>-7.8148571428571447</v>
+        <v>-2.3236000000000008</v>
       </c>
       <c r="E179">
         <f t="shared" si="5"/>
-        <v>0.84334285714285606</v>
+        <v>7.8609999999999989</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
@@ -3276,15 +3287,15 @@
         <v>12.8</v>
       </c>
       <c r="B180">
-        <v>-8.6324699999999996</v>
+        <v>-10.182</v>
       </c>
       <c r="C180">
         <f t="shared" si="4"/>
-        <v>-7.7337142857142869</v>
+        <v>-2.2404000000000011</v>
       </c>
       <c r="E180">
         <f t="shared" si="5"/>
-        <v>0.89875571428571277</v>
+        <v>7.9415999999999993</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
@@ -3292,32 +3303,32 @@
         <v>12.9</v>
       </c>
       <c r="B181">
-        <v>-8.6072399999999991</v>
+        <v>-10.179399999999999</v>
       </c>
       <c r="C181">
         <f t="shared" si="4"/>
-        <v>-7.652571428571429</v>
+        <v>-2.1572000000000013</v>
       </c>
       <c r="E181">
         <f t="shared" si="5"/>
-        <v>0.95466857142857009</v>
+        <v>8.022199999999998</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A182" s="1">
+      <c r="A182" s="2">
         <v>13</v>
       </c>
-      <c r="B182" s="1">
-        <v>-8.5824800000000003</v>
-      </c>
-      <c r="C182" s="1">
-        <f t="shared" si="4"/>
-        <v>-7.571428571428573</v>
-      </c>
-      <c r="D182" s="1"/>
-      <c r="E182" s="1">
-        <f t="shared" si="5"/>
-        <v>1.0110514285714274</v>
+      <c r="B182" s="2">
+        <v>-10.1769</v>
+      </c>
+      <c r="C182" s="2">
+        <f t="shared" si="4"/>
+        <v>-2.0740000000000016</v>
+      </c>
+      <c r="D182" s="2"/>
+      <c r="E182" s="2">
+        <f t="shared" si="5"/>
+        <v>8.1028999999999982</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
@@ -3325,15 +3336,15 @@
         <v>13.1</v>
       </c>
       <c r="B183">
-        <v>-8.5581800000000001</v>
+        <v>-10.174300000000001</v>
       </c>
       <c r="C183">
         <f t="shared" si="4"/>
-        <v>-7.4902857142857169</v>
+        <v>-1.9908000000000019</v>
       </c>
       <c r="E183">
         <f t="shared" si="5"/>
-        <v>1.0678942857142832</v>
+        <v>8.1834999999999987</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
@@ -3341,15 +3352,15 @@
         <v>13.2</v>
       </c>
       <c r="B184">
-        <v>-8.5342699999999994</v>
+        <v>-10.171799999999999</v>
       </c>
       <c r="C184">
         <f t="shared" si="4"/>
-        <v>-7.409142857142859</v>
+        <v>-1.9076000000000022</v>
       </c>
       <c r="E184">
         <f t="shared" si="5"/>
-        <v>1.1251271428571403</v>
+        <v>8.2641999999999971</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
@@ -3357,15 +3368,15 @@
         <v>13.3</v>
       </c>
       <c r="B185">
-        <v>-8.5106900000000003</v>
+        <v>-10.1694</v>
       </c>
       <c r="C185">
         <f t="shared" si="4"/>
-        <v>-7.3280000000000012</v>
+        <v>-1.8244000000000007</v>
       </c>
       <c r="E185">
         <f t="shared" si="5"/>
-        <v>1.1826899999999991</v>
+        <v>8.3449999999999989</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
@@ -3373,15 +3384,15 @@
         <v>13.4</v>
       </c>
       <c r="B186">
-        <v>-8.4876799999999992</v>
+        <v>-10.1669</v>
       </c>
       <c r="C186">
         <f t="shared" si="4"/>
-        <v>-7.2468571428571433</v>
+        <v>-1.741200000000001</v>
       </c>
       <c r="E186">
         <f t="shared" si="5"/>
-        <v>1.2408228571428559</v>
+        <v>8.4256999999999991</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
@@ -3389,15 +3400,15 @@
         <v>13.5</v>
       </c>
       <c r="B187">
-        <v>-8.46509</v>
+        <v>-10.1645</v>
       </c>
       <c r="C187">
         <f t="shared" si="4"/>
-        <v>-7.1657142857142873</v>
+        <v>-1.6580000000000013</v>
       </c>
       <c r="E187">
         <f t="shared" si="5"/>
-        <v>1.2993757142857127</v>
+        <v>8.5064999999999991</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
@@ -3405,15 +3416,15 @@
         <v>13.6</v>
       </c>
       <c r="B188">
-        <v>-8.4428000000000001</v>
+        <v>-10.162000000000001</v>
       </c>
       <c r="C188">
         <f t="shared" si="4"/>
-        <v>-7.0845714285714312</v>
+        <v>-1.5748000000000015</v>
       </c>
       <c r="E188">
         <f t="shared" si="5"/>
-        <v>1.3582285714285689</v>
+        <v>8.5871999999999993</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
@@ -3421,15 +3432,15 @@
         <v>13.7</v>
       </c>
       <c r="B189">
-        <v>-8.4208800000000004</v>
+        <v>-10.159599999999999</v>
       </c>
       <c r="C189">
         <f t="shared" si="4"/>
-        <v>-7.0034285714285733</v>
+        <v>-1.4916000000000018</v>
       </c>
       <c r="E189">
         <f t="shared" si="5"/>
-        <v>1.417451428571427</v>
+        <v>8.6679999999999975</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
@@ -3437,15 +3448,15 @@
         <v>13.8</v>
       </c>
       <c r="B190">
-        <v>-8.3993199999999995</v>
+        <v>-10.157299999999999</v>
       </c>
       <c r="C190">
         <f t="shared" si="4"/>
-        <v>-6.9222857142857155</v>
+        <v>-1.4084000000000003</v>
       </c>
       <c r="E190">
         <f t="shared" si="5"/>
-        <v>1.477034285714284</v>
+        <v>8.748899999999999</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
@@ -3453,15 +3464,15 @@
         <v>13.9</v>
       </c>
       <c r="B191">
-        <v>-8.3781300000000005</v>
+        <v>-10.1549</v>
       </c>
       <c r="C191">
         <f t="shared" si="4"/>
-        <v>-6.8411428571428576</v>
+        <v>-1.3252000000000006</v>
       </c>
       <c r="E191">
         <f t="shared" si="5"/>
-        <v>1.5369871428571429</v>
+        <v>8.829699999999999</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
@@ -3469,15 +3480,15 @@
         <v>14</v>
       </c>
       <c r="B192">
-        <v>-8.3572900000000008</v>
+        <v>-10.1525</v>
       </c>
       <c r="C192">
         <f t="shared" si="4"/>
-        <v>-6.7600000000000016</v>
+        <v>-1.2420000000000009</v>
       </c>
       <c r="E192">
         <f t="shared" si="5"/>
-        <v>1.5972899999999992</v>
+        <v>8.910499999999999</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
@@ -3485,15 +3496,15 @@
         <v>14.1</v>
       </c>
       <c r="B193">
-        <v>-8.3368300000000009</v>
+        <v>-10.1502</v>
       </c>
       <c r="C193">
         <f t="shared" si="4"/>
-        <v>-6.6788571428571455</v>
+        <v>-1.1588000000000012</v>
       </c>
       <c r="E193">
         <f t="shared" si="5"/>
-        <v>1.6579728571428554</v>
+        <v>8.9913999999999987</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.3">
@@ -3501,15 +3512,15 @@
         <v>14.2</v>
       </c>
       <c r="B194">
-        <v>-8.3167100000000005</v>
+        <v>-10.1479</v>
       </c>
       <c r="C194">
         <f t="shared" si="4"/>
-        <v>-6.5977142857142876</v>
+        <v>-1.0756000000000014</v>
       </c>
       <c r="E194">
         <f t="shared" si="5"/>
-        <v>1.7189957142857129</v>
+        <v>9.0722999999999985</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
@@ -3517,15 +3528,15 @@
         <v>14.3</v>
       </c>
       <c r="B195">
-        <v>-8.2969600000000003</v>
+        <v>-10.1456</v>
       </c>
       <c r="C195">
-        <f t="shared" ref="C195:C252" si="6">((142/175)*A195) -18.12</f>
-        <v>-6.5165714285714298</v>
+        <f t="shared" ref="C195:C252" si="6">((104/125)*A195) -12.89</f>
+        <v>-0.99239999999999995</v>
       </c>
       <c r="E195">
         <f t="shared" ref="E195:E252" si="7">C195-B195</f>
-        <v>1.7803885714285705</v>
+        <v>9.1532</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
@@ -3533,15 +3544,15 @@
         <v>14.4</v>
       </c>
       <c r="B196">
-        <v>-8.2775700000000008</v>
+        <v>-10.1433</v>
       </c>
       <c r="C196">
         <f t="shared" si="6"/>
-        <v>-6.4354285714285719</v>
+        <v>-0.90920000000000023</v>
       </c>
       <c r="E196">
         <f t="shared" si="7"/>
-        <v>1.8421414285714288</v>
+        <v>9.2340999999999998</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
@@ -3549,16 +3560,16 @@
         <v>14.5</v>
       </c>
       <c r="B197" s="2">
-        <v>-8.2585499999999996</v>
-      </c>
-      <c r="C197" s="2">
-        <f t="shared" si="6"/>
-        <v>-6.3542857142857159</v>
+        <v>-10.141</v>
+      </c>
+      <c r="C197">
+        <f t="shared" si="6"/>
+        <v>-0.82600000000000051</v>
       </c>
       <c r="D197" s="2"/>
       <c r="E197" s="2">
         <f t="shared" si="7"/>
-        <v>1.9042642857142837</v>
+        <v>9.3149999999999995</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.3">
@@ -3566,15 +3577,15 @@
         <v>14.6</v>
       </c>
       <c r="B198">
-        <v>-8.2398699999999998</v>
+        <v>-10.1387</v>
       </c>
       <c r="C198">
         <f t="shared" si="6"/>
-        <v>-6.2731428571428598</v>
+        <v>-0.74280000000000079</v>
       </c>
       <c r="E198">
         <f t="shared" si="7"/>
-        <v>1.96672714285714</v>
+        <v>9.3958999999999993</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.3">
@@ -3582,15 +3593,15 @@
         <v>14.7</v>
       </c>
       <c r="B199">
-        <v>-8.2216000000000005</v>
+        <v>-10.1364</v>
       </c>
       <c r="C199">
         <f t="shared" si="6"/>
-        <v>-6.1920000000000019</v>
+        <v>-0.65960000000000107</v>
       </c>
       <c r="E199">
         <f t="shared" si="7"/>
-        <v>2.0295999999999985</v>
+        <v>9.476799999999999</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.3">
@@ -3598,15 +3609,15 @@
         <v>14.8</v>
       </c>
       <c r="B200">
-        <v>-8.2036999999999995</v>
+        <v>-10.1342</v>
       </c>
       <c r="C200">
         <f t="shared" si="6"/>
-        <v>-6.1108571428571441</v>
+        <v>-0.57640000000000136</v>
       </c>
       <c r="E200">
         <f t="shared" si="7"/>
-        <v>2.0928428571428555</v>
+        <v>9.5577999999999985</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.3">
@@ -3614,15 +3625,15 @@
         <v>14.9</v>
       </c>
       <c r="B201">
-        <v>-8.1861700000000006</v>
+        <v>-10.1319</v>
       </c>
       <c r="C201">
         <f t="shared" si="6"/>
-        <v>-6.0297142857142862</v>
+        <v>-0.49320000000000164</v>
       </c>
       <c r="E201">
         <f t="shared" si="7"/>
-        <v>2.1564557142857144</v>
+        <v>9.6386999999999983</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.3">
@@ -3630,15 +3641,15 @@
         <v>15</v>
       </c>
       <c r="B202">
-        <v>-8.1690299999999993</v>
+        <v>-10.1297</v>
       </c>
       <c r="C202">
         <f t="shared" si="6"/>
-        <v>-5.9485714285714302</v>
+        <v>-0.41000000000000192</v>
       </c>
       <c r="E202">
         <f t="shared" si="7"/>
-        <v>2.2204585714285692</v>
+        <v>9.7196999999999978</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.3">
@@ -3646,15 +3657,15 @@
         <v>15.1</v>
       </c>
       <c r="B203">
-        <v>-8.1522799999999993</v>
+        <v>-10.1275</v>
       </c>
       <c r="C203">
         <f t="shared" si="6"/>
-        <v>-5.8674285714285741</v>
+        <v>-0.3268000000000022</v>
       </c>
       <c r="E203">
         <f t="shared" si="7"/>
-        <v>2.2848514285714252</v>
+        <v>9.8006999999999973</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.3">
@@ -3662,15 +3673,15 @@
         <v>15.2</v>
       </c>
       <c r="B204">
-        <v>-8.1359200000000005</v>
+        <v>-10.125299999999999</v>
       </c>
       <c r="C204">
         <f t="shared" si="6"/>
-        <v>-5.7862857142857163</v>
+        <v>-0.24360000000000248</v>
       </c>
       <c r="E204">
         <f t="shared" si="7"/>
-        <v>2.3496342857142842</v>
+        <v>9.8816999999999968</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.3">
@@ -3678,15 +3689,15 @@
         <v>15.3</v>
       </c>
       <c r="B205">
-        <v>-8.1199600000000007</v>
+        <v>-10.123100000000001</v>
       </c>
       <c r="C205">
         <f t="shared" si="6"/>
-        <v>-5.7051428571428584</v>
+        <v>-0.16040000000000099</v>
       </c>
       <c r="E205">
         <f t="shared" si="7"/>
-        <v>2.4148171428571423</v>
+        <v>9.9626999999999999</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.3">
@@ -3694,15 +3705,15 @@
         <v>15.4</v>
       </c>
       <c r="B206">
-        <v>-8.1043900000000004</v>
+        <v>-10.120900000000001</v>
       </c>
       <c r="C206">
         <f t="shared" si="6"/>
-        <v>-5.6240000000000006</v>
+        <v>-7.7200000000001268E-2</v>
       </c>
       <c r="E206">
         <f t="shared" si="7"/>
-        <v>2.4803899999999999</v>
+        <v>10.043699999999999</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.3">
@@ -3710,15 +3721,15 @@
         <v>15.5</v>
       </c>
       <c r="B207">
-        <v>-8.0892099999999996</v>
+        <v>-10.1187</v>
       </c>
       <c r="C207">
         <f t="shared" si="6"/>
-        <v>-5.5428571428571445</v>
+        <v>5.999999999998451E-3</v>
       </c>
       <c r="E207">
         <f t="shared" si="7"/>
-        <v>2.5463528571428551</v>
+        <v>10.124699999999999</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.3">
@@ -3726,15 +3737,15 @@
         <v>15.6</v>
       </c>
       <c r="B208">
-        <v>-8.0744299999999996</v>
+        <v>-10.1165</v>
       </c>
       <c r="C208">
         <f t="shared" si="6"/>
-        <v>-5.4617142857142884</v>
+        <v>8.919999999999817E-2</v>
       </c>
       <c r="E208">
         <f t="shared" si="7"/>
-        <v>2.6127157142857111</v>
+        <v>10.205699999999998</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.3">
@@ -3742,15 +3753,15 @@
         <v>15.7</v>
       </c>
       <c r="B209">
-        <v>-8.0600500000000004</v>
+        <v>-10.1144</v>
       </c>
       <c r="C209">
         <f t="shared" si="6"/>
-        <v>-5.3805714285714306</v>
+        <v>0.17239999999999789</v>
       </c>
       <c r="E209">
         <f t="shared" si="7"/>
-        <v>2.6794785714285698</v>
+        <v>10.286799999999998</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.3">
@@ -3758,15 +3769,15 @@
         <v>15.8</v>
       </c>
       <c r="B210">
-        <v>-8.0460600000000007</v>
+        <v>-10.1122</v>
       </c>
       <c r="C210">
         <f t="shared" si="6"/>
-        <v>-5.2994285714285727</v>
+        <v>0.25559999999999938</v>
       </c>
       <c r="E210">
         <f t="shared" si="7"/>
-        <v>2.7466314285714279</v>
+        <v>10.367799999999999</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.3">
@@ -3774,15 +3785,15 @@
         <v>15.9</v>
       </c>
       <c r="B211">
-        <v>-8.0324500000000008</v>
+        <v>-10.110099999999999</v>
       </c>
       <c r="C211">
         <f t="shared" si="6"/>
-        <v>-5.2182857142857149</v>
+        <v>0.3387999999999991</v>
       </c>
       <c r="E211">
         <f t="shared" si="7"/>
-        <v>2.8141642857142859</v>
+        <v>10.448899999999998</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.3">
@@ -3790,15 +3801,15 @@
         <v>16</v>
       </c>
       <c r="B212">
-        <v>-8.0192200000000007</v>
+        <v>-10.107900000000001</v>
       </c>
       <c r="C212">
         <f t="shared" si="6"/>
-        <v>-5.1371428571428588</v>
+        <v>0.42199999999999882</v>
       </c>
       <c r="E212">
         <f t="shared" si="7"/>
-        <v>2.8820771428571419</v>
+        <v>10.5299</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.3">
@@ -3806,15 +3817,15 @@
         <v>16.100000000000001</v>
       </c>
       <c r="B213">
-        <v>-8.0063700000000004</v>
+        <v>-10.1058</v>
       </c>
       <c r="C213">
         <f t="shared" si="6"/>
-        <v>-5.0560000000000009</v>
+        <v>0.50520000000000032</v>
       </c>
       <c r="E213">
         <f t="shared" si="7"/>
-        <v>2.9503699999999995</v>
+        <v>10.611000000000001</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.3">
@@ -3822,15 +3833,15 @@
         <v>16.2</v>
       </c>
       <c r="B214">
-        <v>-7.9938799999999999</v>
+        <v>-10.1037</v>
       </c>
       <c r="C214">
         <f t="shared" si="6"/>
-        <v>-4.9748571428571449</v>
+        <v>0.58839999999999826</v>
       </c>
       <c r="E214">
         <f t="shared" si="7"/>
-        <v>3.019022857142855</v>
+        <v>10.692099999999998</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.3">
@@ -3838,15 +3849,15 @@
         <v>16.3</v>
       </c>
       <c r="B215">
-        <v>-7.9817600000000004</v>
+        <v>-10.101599999999999</v>
       </c>
       <c r="C215">
         <f t="shared" si="6"/>
-        <v>-4.893714285714287</v>
+        <v>0.67159999999999975</v>
       </c>
       <c r="E215">
         <f t="shared" si="7"/>
-        <v>3.0880457142857134</v>
+        <v>10.773199999999999</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.3">
@@ -3854,15 +3865,15 @@
         <v>16.399999999999999</v>
       </c>
       <c r="B216">
-        <v>-7.9699799999999996</v>
+        <v>-10.099500000000001</v>
       </c>
       <c r="C216">
         <f t="shared" si="6"/>
-        <v>-4.8125714285714309</v>
+        <v>0.75479999999999769</v>
       </c>
       <c r="E216">
         <f t="shared" si="7"/>
-        <v>3.1574085714285687</v>
+        <v>10.854299999999999</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
@@ -3870,15 +3881,15 @@
         <v>16.5</v>
       </c>
       <c r="B217">
-        <v>-7.9585499999999998</v>
+        <v>-10.0975</v>
       </c>
       <c r="C217">
         <f t="shared" si="6"/>
-        <v>-4.7314285714285731</v>
+        <v>0.83799999999999919</v>
       </c>
       <c r="E217">
         <f t="shared" si="7"/>
-        <v>3.2271214285714267</v>
+        <v>10.935499999999999</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.3">
@@ -3886,15 +3897,15 @@
         <v>16.600000000000001</v>
       </c>
       <c r="B218">
-        <v>-7.9474499999999999</v>
+        <v>-10.0954</v>
       </c>
       <c r="C218">
         <f t="shared" si="6"/>
-        <v>-4.6502857142857152</v>
+        <v>0.92120000000000068</v>
       </c>
       <c r="E218">
         <f t="shared" si="7"/>
-        <v>3.2971642857142847</v>
+        <v>11.0166</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
@@ -3902,15 +3913,15 @@
         <v>16.7</v>
       </c>
       <c r="B219">
-        <v>-7.93668</v>
+        <v>-10.093400000000001</v>
       </c>
       <c r="C219">
         <f t="shared" si="6"/>
-        <v>-4.5691428571428592</v>
+        <v>1.0043999999999986</v>
       </c>
       <c r="E219">
         <f t="shared" si="7"/>
-        <v>3.3675371428571408</v>
+        <v>11.097799999999999</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.3">
@@ -3918,15 +3929,15 @@
         <v>16.8</v>
       </c>
       <c r="B220">
-        <v>-7.9262300000000003</v>
+        <v>-10.0914</v>
       </c>
       <c r="C220">
         <f t="shared" si="6"/>
-        <v>-4.4880000000000013</v>
+        <v>1.0876000000000001</v>
       </c>
       <c r="E220">
         <f t="shared" si="7"/>
-        <v>3.438229999999999</v>
+        <v>11.179</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.3">
@@ -3934,15 +3945,15 @@
         <v>16.899999999999999</v>
       </c>
       <c r="B221">
-        <v>-7.9160899999999996</v>
+        <v>-10.089399999999999</v>
       </c>
       <c r="C221">
         <f t="shared" si="6"/>
-        <v>-4.4068571428571452</v>
+        <v>1.1707999999999981</v>
       </c>
       <c r="E221">
         <f t="shared" si="7"/>
-        <v>3.5092328571428544</v>
+        <v>11.260199999999998</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
@@ -3950,15 +3961,15 @@
         <v>17</v>
       </c>
       <c r="B222">
-        <v>-7.90625</v>
+        <v>-10.087400000000001</v>
       </c>
       <c r="C222">
         <f t="shared" si="6"/>
-        <v>-4.3257142857142874</v>
+        <v>1.2539999999999996</v>
       </c>
       <c r="E222">
         <f t="shared" si="7"/>
-        <v>3.5805357142857126</v>
+        <v>11.3414</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
@@ -3966,15 +3977,15 @@
         <v>17.100000000000001</v>
       </c>
       <c r="B223">
-        <v>-7.8967099999999997</v>
+        <v>-10.0854</v>
       </c>
       <c r="C223">
         <f t="shared" si="6"/>
-        <v>-4.2445714285714295</v>
+        <v>1.3371999999999993</v>
       </c>
       <c r="E223">
         <f t="shared" si="7"/>
-        <v>3.6521385714285701</v>
+        <v>11.422599999999999</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.3">
@@ -3982,15 +3993,15 @@
         <v>17.2</v>
       </c>
       <c r="B224">
-        <v>-7.8874500000000003</v>
+        <v>-10.083500000000001</v>
       </c>
       <c r="C224">
         <f t="shared" si="6"/>
-        <v>-4.1634285714285735</v>
+        <v>1.420399999999999</v>
       </c>
       <c r="E224">
         <f t="shared" si="7"/>
-        <v>3.7240214285714268</v>
+        <v>11.5039</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.3">
@@ -3998,15 +4009,15 @@
         <v>17.3</v>
       </c>
       <c r="B225">
-        <v>-7.8784700000000001</v>
+        <v>-10.0816</v>
       </c>
       <c r="C225">
         <f t="shared" si="6"/>
-        <v>-4.0822857142857156</v>
+        <v>1.5035999999999987</v>
       </c>
       <c r="E225">
         <f t="shared" si="7"/>
-        <v>3.7961842857142845</v>
+        <v>11.585199999999999</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.3">
@@ -4014,15 +4025,15 @@
         <v>17.399999999999999</v>
       </c>
       <c r="B226">
-        <v>-7.8697600000000003</v>
+        <v>-10.079700000000001</v>
       </c>
       <c r="C226">
         <f t="shared" si="6"/>
-        <v>-4.0011428571428596</v>
+        <v>1.5867999999999984</v>
       </c>
       <c r="E226">
         <f t="shared" si="7"/>
-        <v>3.8686171428571408</v>
+        <v>11.666499999999999</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.3">
@@ -4030,15 +4041,15 @@
         <v>17.5</v>
       </c>
       <c r="B227">
-        <v>-7.8613200000000001</v>
+        <v>-10.0778</v>
       </c>
       <c r="C227">
         <f t="shared" si="6"/>
-        <v>-3.9200000000000017</v>
+        <v>1.6699999999999982</v>
       </c>
       <c r="E227">
         <f t="shared" si="7"/>
-        <v>3.9413199999999984</v>
+        <v>11.747799999999998</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.3">
@@ -4046,15 +4057,15 @@
         <v>17.600000000000001</v>
       </c>
       <c r="B228">
-        <v>-7.8531300000000002</v>
+        <v>-10.076000000000001</v>
       </c>
       <c r="C228">
         <f t="shared" si="6"/>
-        <v>-3.8388571428571439</v>
+        <v>1.7531999999999996</v>
       </c>
       <c r="E228">
         <f t="shared" si="7"/>
-        <v>4.0142728571428563</v>
+        <v>11.8292</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.3">
@@ -4062,15 +4073,15 @@
         <v>17.7</v>
       </c>
       <c r="B229">
-        <v>-7.8451899999999997</v>
+        <v>-10.074199999999999</v>
       </c>
       <c r="C229">
         <f t="shared" si="6"/>
-        <v>-3.7577142857142878</v>
+        <v>1.8363999999999976</v>
       </c>
       <c r="E229">
         <f t="shared" si="7"/>
-        <v>4.0874757142857119</v>
+        <v>11.910599999999997</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.3">
@@ -4078,15 +4089,15 @@
         <v>17.8</v>
       </c>
       <c r="B230">
-        <v>-7.8375000000000004</v>
+        <v>-10.0724</v>
       </c>
       <c r="C230">
         <f t="shared" si="6"/>
-        <v>-3.6765714285714299</v>
+        <v>1.9195999999999991</v>
       </c>
       <c r="E230">
         <f t="shared" si="7"/>
-        <v>4.1609285714285704</v>
+        <v>11.991999999999999</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.3">
@@ -4094,15 +4105,15 @@
         <v>17.899999999999999</v>
       </c>
       <c r="B231">
-        <v>-7.8300400000000003</v>
+        <v>-10.070600000000001</v>
       </c>
       <c r="C231">
         <f t="shared" si="6"/>
-        <v>-3.5954285714285739</v>
+        <v>2.002799999999997</v>
       </c>
       <c r="E231">
         <f t="shared" si="7"/>
-        <v>4.2346114285714265</v>
+        <v>12.073399999999998</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.3">
@@ -4110,15 +4121,15 @@
         <v>18</v>
       </c>
       <c r="B232">
-        <v>-7.8228099999999996</v>
+        <v>-10.068899999999999</v>
       </c>
       <c r="C232">
         <f t="shared" si="6"/>
-        <v>-3.514285714285716</v>
+        <v>2.0859999999999985</v>
       </c>
       <c r="E232">
         <f t="shared" si="7"/>
-        <v>4.3085242857142836</v>
+        <v>12.154899999999998</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.3">
@@ -4126,15 +4137,15 @@
         <v>18.100000000000001</v>
       </c>
       <c r="B233">
-        <v>-7.8158000000000003</v>
+        <v>-10.0672</v>
       </c>
       <c r="C233">
         <f t="shared" si="6"/>
-        <v>-3.4331428571428582</v>
+        <v>2.1692</v>
       </c>
       <c r="E233">
         <f t="shared" si="7"/>
-        <v>4.3826571428571421</v>
+        <v>12.2364</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.3">
@@ -4142,15 +4153,15 @@
         <v>18.2</v>
       </c>
       <c r="B234">
-        <v>-7.8090000000000002</v>
+        <v>-10.0656</v>
       </c>
       <c r="C234">
         <f t="shared" si="6"/>
-        <v>-3.3520000000000021</v>
+        <v>2.252399999999998</v>
       </c>
       <c r="E234">
         <f t="shared" si="7"/>
-        <v>4.4569999999999981</v>
+        <v>12.317999999999998</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.3">
@@ -4158,15 +4169,15 @@
         <v>18.3</v>
       </c>
       <c r="B235">
-        <v>-7.8024199999999997</v>
+        <v>-10.0639</v>
       </c>
       <c r="C235">
         <f t="shared" si="6"/>
-        <v>-3.2708571428571442</v>
+        <v>2.3355999999999995</v>
       </c>
       <c r="E235">
         <f t="shared" si="7"/>
-        <v>4.5315628571428554</v>
+        <v>12.3995</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.3">
@@ -4174,15 +4185,15 @@
         <v>18.399999999999999</v>
       </c>
       <c r="B236">
-        <v>-7.7960399999999996</v>
+        <v>-10.0623</v>
       </c>
       <c r="C236">
         <f t="shared" si="6"/>
-        <v>-3.1897142857142882</v>
+        <v>2.4187999999999974</v>
       </c>
       <c r="E236">
         <f t="shared" si="7"/>
-        <v>4.6063257142857115</v>
+        <v>12.481099999999998</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.3">
@@ -4190,15 +4201,15 @@
         <v>18.5</v>
       </c>
       <c r="B237">
-        <v>-7.7898399999999999</v>
+        <v>-10.0608</v>
       </c>
       <c r="C237">
         <f t="shared" si="6"/>
-        <v>-3.1085714285714303</v>
+        <v>2.5019999999999989</v>
       </c>
       <c r="E237">
         <f t="shared" si="7"/>
-        <v>4.6812685714285696</v>
+        <v>12.562799999999999</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.3">
@@ -4206,15 +4217,15 @@
         <v>18.600000000000001</v>
       </c>
       <c r="B238">
-        <v>-7.7838399999999996</v>
+        <v>-10.0593</v>
       </c>
       <c r="C238">
         <f t="shared" si="6"/>
-        <v>-3.0274285714285725</v>
+        <v>2.5852000000000004</v>
       </c>
       <c r="E238">
         <f t="shared" si="7"/>
-        <v>4.7564114285714272</v>
+        <v>12.644500000000001</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.3">
@@ -4222,15 +4233,15 @@
         <v>18.7</v>
       </c>
       <c r="B239">
-        <v>-7.7780199999999997</v>
+        <v>-10.0578</v>
       </c>
       <c r="C239">
         <f t="shared" si="6"/>
-        <v>-2.9462857142857164</v>
+        <v>2.6683999999999983</v>
       </c>
       <c r="E239">
         <f t="shared" si="7"/>
-        <v>4.8317342857142833</v>
+        <v>12.726199999999999</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.3">
@@ -4238,15 +4249,15 @@
         <v>18.8</v>
       </c>
       <c r="B240">
-        <v>-7.7723500000000003</v>
+        <v>-10.0563</v>
       </c>
       <c r="C240">
         <f t="shared" si="6"/>
-        <v>-2.8651428571428585</v>
+        <v>2.7515999999999998</v>
       </c>
       <c r="E240">
         <f t="shared" si="7"/>
-        <v>4.9072071428571418</v>
+        <v>12.8079</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.3">
@@ -4254,15 +4265,15 @@
         <v>18.899999999999999</v>
       </c>
       <c r="B241">
-        <v>-7.7668799999999996</v>
+        <v>-10.0549</v>
       </c>
       <c r="C241">
         <f t="shared" si="6"/>
-        <v>-2.7840000000000025</v>
+        <v>2.8347999999999978</v>
       </c>
       <c r="E241">
         <f t="shared" si="7"/>
-        <v>4.9828799999999971</v>
+        <v>12.889699999999998</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.3">
@@ -4270,15 +4281,15 @@
         <v>19</v>
       </c>
       <c r="B242">
-        <v>-7.7615499999999997</v>
+        <v>-10.053599999999999</v>
       </c>
       <c r="C242">
         <f t="shared" si="6"/>
-        <v>-2.7028571428571446</v>
+        <v>2.9179999999999993</v>
       </c>
       <c r="E242">
         <f t="shared" si="7"/>
-        <v>5.0586928571428551</v>
+        <v>12.971599999999999</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.3">
@@ -4286,15 +4297,15 @@
         <v>19.100000000000001</v>
       </c>
       <c r="B243">
-        <v>-7.7563700000000004</v>
+        <v>-10.052300000000001</v>
       </c>
       <c r="C243">
         <f t="shared" si="6"/>
-        <v>-2.6217142857142868</v>
+        <v>3.0012000000000008</v>
       </c>
       <c r="E243">
         <f t="shared" si="7"/>
-        <v>5.1346557142857137</v>
+        <v>13.053500000000001</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.3">
@@ -4302,15 +4313,15 @@
         <v>19.2</v>
       </c>
       <c r="B244">
-        <v>-7.7513399999999999</v>
+        <v>-10.051</v>
       </c>
       <c r="C244">
         <f t="shared" si="6"/>
-        <v>-2.5405714285714307</v>
+        <v>3.0843999999999987</v>
       </c>
       <c r="E244">
         <f t="shared" si="7"/>
-        <v>5.2107685714285692</v>
+        <v>13.135399999999999</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.3">
@@ -4318,15 +4329,15 @@
         <v>19.3</v>
       </c>
       <c r="B245">
-        <v>-7.7464500000000003</v>
+        <v>-10.049799999999999</v>
       </c>
       <c r="C245">
         <f t="shared" si="6"/>
-        <v>-2.4594285714285729</v>
+        <v>3.1676000000000002</v>
       </c>
       <c r="E245">
         <f t="shared" si="7"/>
-        <v>5.2870214285714274</v>
+        <v>13.2174</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.3">
@@ -4334,15 +4345,15 @@
         <v>19.399999999999999</v>
       </c>
       <c r="B246">
-        <v>-7.7416999999999998</v>
+        <v>-10.0486</v>
       </c>
       <c r="C246">
         <f t="shared" si="6"/>
-        <v>-2.3782857142857168</v>
+        <v>3.2507999999999981</v>
       </c>
       <c r="E246">
         <f t="shared" si="7"/>
-        <v>5.363414285714283</v>
+        <v>13.299399999999999</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.3">
@@ -4350,15 +4361,15 @@
         <v>19.5</v>
       </c>
       <c r="B247">
-        <v>-7.7370700000000001</v>
+        <v>-10.0474</v>
       </c>
       <c r="C247">
         <f t="shared" si="6"/>
-        <v>-2.2971428571428589</v>
+        <v>3.3339999999999996</v>
       </c>
       <c r="E247">
         <f t="shared" si="7"/>
-        <v>5.4399271428571412</v>
+        <v>13.381399999999999</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.3">
@@ -4366,15 +4377,15 @@
         <v>19.600000000000001</v>
       </c>
       <c r="B248">
-        <v>-7.7325699999999999</v>
+        <v>-10.0463</v>
       </c>
       <c r="C248">
         <f t="shared" si="6"/>
-        <v>-2.2160000000000011</v>
+        <v>3.4172000000000011</v>
       </c>
       <c r="E248">
         <f t="shared" si="7"/>
-        <v>5.5165699999999989</v>
+        <v>13.463500000000002</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.3">
@@ -4382,15 +4393,15 @@
         <v>19.7</v>
       </c>
       <c r="B249">
-        <v>-7.72818</v>
+        <v>-10.045299999999999</v>
       </c>
       <c r="C249">
         <f t="shared" si="6"/>
-        <v>-2.134857142857145</v>
+        <v>3.5003999999999991</v>
       </c>
       <c r="E249">
         <f t="shared" si="7"/>
-        <v>5.593322857142855</v>
+        <v>13.545699999999998</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.3">
@@ -4398,15 +4409,15 @@
         <v>19.8</v>
       </c>
       <c r="B250">
-        <v>-7.7239100000000001</v>
+        <v>-10.0442</v>
       </c>
       <c r="C250">
         <f t="shared" si="6"/>
-        <v>-2.0537142857142854</v>
+        <v>3.5836000000000006</v>
       </c>
       <c r="E250">
         <f t="shared" si="7"/>
-        <v>5.6701957142857147</v>
+        <v>13.627800000000001</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.3">
@@ -4414,15 +4425,15 @@
         <v>19.899999999999999</v>
       </c>
       <c r="B251">
-        <v>-7.7197399999999998</v>
+        <v>-10.0433</v>
       </c>
       <c r="C251">
         <f t="shared" si="6"/>
-        <v>-1.9725714285714311</v>
+        <v>3.6667999999999985</v>
       </c>
       <c r="E251">
         <f t="shared" si="7"/>
-        <v>5.7471685714285687</v>
+        <v>13.710099999999999</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.3">
@@ -4430,18 +4441,19 @@
         <v>20</v>
       </c>
       <c r="B252">
-        <v>-7.7156700000000003</v>
+        <v>-10.042299999999999</v>
       </c>
       <c r="C252">
         <f t="shared" si="6"/>
-        <v>-1.8914285714285732</v>
+        <v>3.75</v>
       </c>
       <c r="E252">
         <f t="shared" si="7"/>
-        <v>5.824241428571427</v>
+        <v>13.792299999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>